<commit_message>
Work completed on StudentInfo_df file
Work included .. a copy python notebook / removal of other csv files / removal of columns / one-hot encoding of variables / run of logistic regression to test accuracy of the model
</commit_message>
<xml_diff>
--- a/Table of article comparision.xlsx
+++ b/Table of article comparision.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c49cb972183112a/Documents OneDrive/06 - CCT Masters in DA/Capstone - 2023/Capstone_Project_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FFAAB33-7800-43FD-B24F-F34C11421AA3}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E738FDC-4EA1-4A60-89FA-3935008A3CCC}"/>
   <bookViews>
     <workbookView xWindow="28920" yWindow="60" windowWidth="13950" windowHeight="15690" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
   <si>
     <t>Authors</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t>Causal discovery / causal algorithms</t>
+  </si>
+  <si>
+    <t>Al-azazi &amp; Ghurab 2022</t>
+  </si>
+  <si>
+    <t>ANN-LSTM</t>
   </si>
 </sst>
 </file>
@@ -589,8 +595,8 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,9 +891,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Algorithm 2 - Decision Tree
Initial work on Algorithm 2 and working with feature selection to improve accuracy
</commit_message>
<xml_diff>
--- a/Table of article comparision.xlsx
+++ b/Table of article comparision.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c49cb972183112a/Documents OneDrive/06 - CCT Masters in DA/Capstone - 2023/Capstone_Project_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E738FDC-4EA1-4A60-89FA-3935008A3CCC}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E1CDCE7-4757-49D5-9E93-0918D101836A}"/>
   <bookViews>
-    <workbookView xWindow="28920" yWindow="60" windowWidth="13950" windowHeight="15690" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
+    <workbookView xWindow="28950" yWindow="180" windowWidth="13950" windowHeight="15405" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Algorithm Results" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="77">
   <si>
     <t>Authors</t>
   </si>
@@ -92,9 +93,6 @@
     <t>Assessment Score / Final Results / Educat Level</t>
   </si>
   <si>
-    <t xml:space="preserve">J48 / Decision Tree / JRIP / Gradient-boosted Classifiers </t>
-  </si>
-  <si>
     <t>Dependent Var</t>
   </si>
   <si>
@@ -204,13 +202,79 @@
   </si>
   <si>
     <t>ANN-LSTM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J48 Decision Tree / JRIP / Gradient-boosted Classifiers </t>
+  </si>
+  <si>
+    <t>Algorithm 1</t>
+  </si>
+  <si>
+    <t>Logistic Regression</t>
+  </si>
+  <si>
+    <t>Initial Result</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Train</t>
+  </si>
+  <si>
+    <t>With GridSearch CV</t>
+  </si>
+  <si>
+    <t>Algorithm 2</t>
+  </si>
+  <si>
+    <t>Decision Tree</t>
+  </si>
+  <si>
+    <t>Test Accuracy</t>
+  </si>
+  <si>
+    <t>with FeatureSelection</t>
+  </si>
+  <si>
+    <t>GridSearch CV - attempt 1</t>
+  </si>
+  <si>
+    <t>GridSearch CV - attempt 2</t>
+  </si>
+  <si>
+    <t>GridSearch CV - attempt 3</t>
+  </si>
+  <si>
+    <t>GridSearch CV - attempt 4</t>
+  </si>
+  <si>
+    <t>@ 1 Feature selected</t>
+  </si>
+  <si>
+    <t>@ 5 Features selected</t>
+  </si>
+  <si>
+    <t>@ 10 Features selected</t>
+  </si>
+  <si>
+    <t>@ 15 Features selected</t>
+  </si>
+  <si>
+    <t>@ 7 Features selected</t>
+  </si>
+  <si>
+    <t>@ 6 Features selected</t>
+  </si>
+  <si>
+    <t>@ 4 Features selected</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,13 +297,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -254,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -271,6 +347,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,9 +678,9 @@
   </sheetPr>
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +717,7 @@
         <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>15</v>
@@ -687,7 +771,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -696,10 +780,10 @@
         <v>4</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>14</v>
@@ -716,7 +800,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>8</v>
@@ -725,13 +809,13 @@
         <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="3">
         <v>0.8</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -739,7 +823,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>8</v>
@@ -748,13 +832,13 @@
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -762,7 +846,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>8</v>
@@ -771,10 +855,10 @@
         <v>4</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -782,7 +866,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>8</v>
@@ -791,7 +875,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -799,19 +883,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -819,19 +903,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -839,19 +923,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -859,16 +943,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -876,19 +960,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -896,10 +980,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -937,20 +1021,206 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>33</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="89" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61403218-7A3E-4B26-8B7C-D3F4D407424F}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3">
+        <v>0.62091499999999999</v>
+      </c>
+      <c r="D3">
+        <v>0.57142899999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5">
+        <v>0.62091499999999999</v>
+      </c>
+      <c r="D5">
+        <v>0.57142899999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6">
+        <v>0.62091499999999999</v>
+      </c>
+      <c r="D6">
+        <v>0.57142899999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7">
+        <v>0.62091499999999999</v>
+      </c>
+      <c r="D7">
+        <v>0.57142899999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8">
+        <v>0.62091499999999999</v>
+      </c>
+      <c r="D8">
+        <v>0.57142899999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12">
+        <v>0.53246753000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14">
+        <v>0.61038899999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15">
+        <v>0.57142857000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16">
+        <v>0.53246753199999997</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17">
+        <v>0.54545454000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18">
+        <v>0.58441558439999997</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0.62337662329999999</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20">
+        <v>0.62337662329999999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="7"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="7"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Algorithm 3 - SVMs
creation of 3 python files to complete SVM + SVM with GridSearch CV + SVM with GridSearch CV &  pram_grid
</commit_message>
<xml_diff>
--- a/Table of article comparision.xlsx
+++ b/Table of article comparision.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c49cb972183112a/Documents OneDrive/06 - CCT Masters in DA/Capstone - 2023/Capstone_Project_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E1CDCE7-4757-49D5-9E93-0918D101836A}"/>
+  <xr:revisionPtr revIDLastSave="235" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8924144-B488-491C-994D-0F0D15761035}"/>
   <bookViews>
-    <workbookView xWindow="28950" yWindow="180" windowWidth="13950" windowHeight="15405" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
+    <workbookView xWindow="30" yWindow="135" windowWidth="13950" windowHeight="15405" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Comparison Chart" sheetId="1" r:id="rId1"/>
     <sheet name="Algorithm Results" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="89">
   <si>
     <t>Authors</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Kohnke et al 2022</t>
   </si>
   <si>
-    <t>Logistic Regression + 10-Fold Validation</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bespoke </t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>Focus on STEM</t>
   </si>
   <si>
-    <t>5-fold cross validation +SVC rbf algorithm</t>
-  </si>
-  <si>
     <t>Votto et al 2021</t>
   </si>
   <si>
@@ -204,9 +198,6 @@
     <t>ANN-LSTM</t>
   </si>
   <si>
-    <t xml:space="preserve">J48 Decision Tree / JRIP / Gradient-boosted Classifiers </t>
-  </si>
-  <si>
     <t>Algorithm 1</t>
   </si>
   <si>
@@ -228,9 +219,6 @@
     <t>Algorithm 2</t>
   </si>
   <si>
-    <t>Decision Tree</t>
-  </si>
-  <si>
     <t>Test Accuracy</t>
   </si>
   <si>
@@ -268,6 +256,121 @@
   </si>
   <si>
     <t>@ 4 Features selected</t>
+  </si>
+  <si>
+    <t>Decision Tree - ungrouped Tenure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decision Tree - grouped tenure </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">J48 Decision Tree </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">/ JRIP / Gradient-boosted Classifiers </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">5-fold cross validation </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+SVC rbf algorithm</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Logistic Regression</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10-Fold Validation</t>
+    </r>
+  </si>
+  <si>
+    <t>Algorithm 3</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>Linear</t>
+  </si>
+  <si>
+    <t>rbf</t>
+  </si>
+  <si>
+    <t>ploy</t>
+  </si>
+  <si>
+    <t>sigmoid</t>
+  </si>
+  <si>
+    <t>with GridSearch CV + rbf</t>
+  </si>
+  <si>
+    <t>with GridSearch CV + param_grid</t>
+  </si>
+  <si>
+    <t>with Hyperparm Tuning</t>
+  </si>
+  <si>
+    <t>Target Var</t>
+  </si>
+  <si>
+    <t>Studied Credits</t>
   </si>
 </sst>
 </file>
@@ -330,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -355,6 +458,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -680,7 +784,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,13 +818,13 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -754,16 +858,16 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="F3" s="4">
         <v>0.80700000000000005</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -771,7 +875,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -780,19 +884,19 @@
         <v>4</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -800,22 +904,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="3">
         <v>0.8</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -823,7 +927,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>8</v>
@@ -832,13 +936,13 @@
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -846,7 +950,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>8</v>
@@ -855,10 +959,10 @@
         <v>4</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -866,7 +970,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>8</v>
@@ -874,8 +978,8 @@
       <c r="D8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>35</v>
+      <c r="E8" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -883,19 +987,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -903,19 +1007,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -923,19 +1027,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="D11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -943,16 +1047,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -960,19 +1064,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -980,10 +1084,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1021,16 +1125,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1041,37 +1145,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61403218-7A3E-4B26-8B7C-D3F4D407424F}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="B1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C2" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C3">
         <v>0.62091499999999999</v>
@@ -1082,12 +1191,12 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C5">
         <v>0.62091499999999999</v>
@@ -1098,7 +1207,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C6">
         <v>0.62091499999999999</v>
@@ -1109,7 +1218,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C7">
         <v>0.62091499999999999</v>
@@ -1120,7 +1229,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C8">
         <v>0.62091499999999999</v>
@@ -1131,21 +1240,24 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>87</v>
+      </c>
       <c r="C11" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C12">
         <v>0.53246753000000002</v>
@@ -1153,12 +1265,12 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C14">
         <v>0.61038899999999996</v>
@@ -1166,7 +1278,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C15">
         <v>0.57142857000000002</v>
@@ -1174,49 +1286,167 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C16">
         <v>0.53246753199999997</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C17">
         <v>0.54545454000000004</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C18">
         <v>0.58441558439999997</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C19" s="9">
         <v>0.62337662329999999</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C20">
         <v>0.62337662329999999</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25">
+        <v>0.62337662329999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26">
+        <v>0.61038899999999996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27">
+        <v>0.57142857000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32">
+        <v>0.68831168831099998</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33">
+        <v>0.70129870129799998</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34">
+        <v>0.70129870129799998</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35">
+        <v>0.70129870129799998</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37">
+        <v>0.70129871097999996</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38">
+        <v>0.70129871097999996</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Algorithm 5 - MLP data
work on two different versions of the algorithm using MLP
</commit_message>
<xml_diff>
--- a/Table of article comparision.xlsx
+++ b/Table of article comparision.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c49cb972183112a/Documents OneDrive/06 - CCT Masters in DA/Capstone - 2023/Capstone_Project_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="290" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21C2A61A-764E-4E78-92E2-0F9DDB301EA6}"/>
+  <xr:revisionPtr revIDLastSave="326" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30AC3093-6150-4297-847D-810B339F3244}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="135" windowWidth="13950" windowHeight="15405" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
+    <workbookView xWindow="30" yWindow="135" windowWidth="13950" windowHeight="15405" firstSheet="1" activeTab="2" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison Chart" sheetId="1" r:id="rId1"/>
     <sheet name="Algorithm Results" sheetId="2" r:id="rId2"/>
+    <sheet name="Algorithm 5 - MLP" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="184">
   <si>
     <t>Authors</t>
   </si>
@@ -393,15 +394,279 @@
   <si>
     <t>`@200 trees</t>
   </si>
+  <si>
+    <t>Algorithm 5</t>
+  </si>
+  <si>
+    <t>MLP - Sequential</t>
+  </si>
+  <si>
+    <t>Epoch 1/10</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 4ms/step - loss: -242081424.0000 - accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 2/10</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 3ms/step - loss: -283053568.0000 - accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 3/10</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 5ms/step - loss: -329420064.0000 - accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 4/10</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 4ms/step - loss: -383456384.0000 - accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 5/10</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 4ms/step - loss: -443147296.0000 - accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 6/10</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 4ms/step - loss: -509580640.0000 - accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 7/10</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 4ms/step - loss: -587204160.0000 - accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 8/10</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 5ms/step - loss: -667973120.0000 - accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 9/10</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 4ms/step - loss: -764345728.0000 - accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 10/10</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 4ms/step - loss: -866226176.0000 - accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial Test - 2 hidden layers </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test 2 </t>
+  </si>
+  <si>
+    <t>Initial Test - 2 hidden layers  with relu and sigmoid as the activation layer</t>
+  </si>
+  <si>
+    <t>Studiet Credits as dependant layer .. Loss function = binary_crossentropy and optimizer = adam</t>
+  </si>
+  <si>
+    <t>Epoch 1/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 13ms/step - loss: -25394743296.0000 - accuracy: 0.0000e+00 - val_loss: -24771162112.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 2/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 8ms/step - loss: -26108925952.0000 - accuracy: 0.0000e+00 - val_loss: -25442850816.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 3/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 8ms/step - loss: -26816679936.0000 - accuracy: 0.0000e+00 - val_loss: -26138527744.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 4/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 9ms/step - loss: -27543879680.0000 - accuracy: 0.0000e+00 - val_loss: -26850807808.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 5/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 8ms/step - loss: -28280655872.0000 - accuracy: 0.0000e+00 - val_loss: -27573581824.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 6/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 8ms/step - loss: -29059145728.0000 - accuracy: 0.0000e+00 - val_loss: -28300064768.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 7/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 8ms/step - loss: -29805772800.0000 - accuracy: 0.0000e+00 - val_loss: -29048614912.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 8/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 8ms/step - loss: -30605600768.0000 - accuracy: 0.0000e+00 - val_loss: -29793935360.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 9/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 8ms/step - loss: -31385100288.0000 - accuracy: 0.0000e+00 - val_loss: -30564853760.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 10/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 8ms/step - loss: -32193349632.0000 - accuracy: 0.0000e+00 - val_loss: -31354171392.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 11/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 11ms/step - loss: -33020014592.0000 - accuracy: 0.0000e+00 - val_loss: -32140675072.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 12/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 9ms/step - loss: -33841115136.0000 - accuracy: 0.0000e+00 - val_loss: -32941174784.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 13/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 12ms/step - loss: -34674659328.0000 - accuracy: 0.0000e+00 - val_loss: -33758574592.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 14/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 8ms/step - loss: -35518062592.0000 - accuracy: 0.0000e+00 - val_loss: -34595278848.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 15/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 9ms/step - loss: -36400070656.0000 - accuracy: 0.0000e+00 - val_loss: -35426832384.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 16/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 9ms/step - loss: -37296611328.0000 - accuracy: 0.0000e+00 - val_loss: -36265394176.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 17/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 10ms/step - loss: -38146936832.0000 - accuracy: 0.0000e+00 - val_loss: -37156323328.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 18/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 9ms/step - loss: -39079579648.0000 - accuracy: 0.0000e+00 - val_loss: -38033629184.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 19/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 8ms/step - loss: -39998951424.0000 - accuracy: 0.0000e+00 - val_loss: -38920065024.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 20/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 9ms/step - loss: -40929095680.0000 - accuracy: 0.0000e+00 - val_loss: -39829299200.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 21/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 9ms/step - loss: -41876824064.0000 - accuracy: 0.0000e+00 - val_loss: -40747204608.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 22/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 9ms/step - loss: -42839941120.0000 - accuracy: 0.0000e+00 - val_loss: -41662656512.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 23/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 8ms/step - loss: -43813273600.0000 - accuracy: 0.0000e+00 - val_loss: -42587631616.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 24/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 9ms/step - loss: -44752834560.0000 - accuracy: 0.0000e+00 - val_loss: -43560857600.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 25/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 9ms/step - loss: -45789294592.0000 - accuracy: 0.0000e+00 - val_loss: -44508856320.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 26/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 10ms/step - loss: -46798168064.0000 - accuracy: 0.0000e+00 - val_loss: -45485510656.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 27/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 10ms/step - loss: -47796768768.0000 - accuracy: 0.0000e+00 - val_loss: -46478618624.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 28/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 10ms/step - loss: -48838012928.0000 - accuracy: 0.0000e+00 - val_loss: -47475539968.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 29/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 9ms/step - loss: -49879625728.0000 - accuracy: 0.0000e+00 - val_loss: -48487399424.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 30/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 8ms/step - loss: -50940579840.0000 - accuracy: 0.0000e+00 - val_loss: -49510993920.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>2 hidden Layers with relu and sigmoid as the final activation layer</t>
+  </si>
+  <si>
+    <t>Student ID as dependant layer .. Loss function = binary_crossentropy and optimizer = adam</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -430,8 +695,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -441,6 +717,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -537,7 +819,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -570,22 +852,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -602,6 +885,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>466726</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>546984</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>190061</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D75E81F2-3610-537D-C262-BE81D81E7F1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="466726" y="10353675"/>
+          <a:ext cx="5395208" cy="3190436"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -915,7 +1247,7 @@
       <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
@@ -929,7 +1261,7 @@
     <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -955,7 +1287,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -975,7 +1307,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="30">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -998,7 +1330,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="60">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1027,7 +1359,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="30">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1050,7 +1382,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="45">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1073,7 +1405,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="30">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1093,7 +1425,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1110,7 +1442,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="30">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1130,7 +1462,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1150,7 +1482,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1170,7 +1502,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="30">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1187,7 +1519,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="30">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1207,7 +1539,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="30">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1218,37 +1550,37 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1273,13 +1605,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61403218-7A3E-4B26-8B7C-D3F4D407424F}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
@@ -1287,7 +1619,7 @@
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -1295,7 +1627,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="6" t="s">
         <v>82</v>
       </c>
@@ -1306,7 +1638,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="B3" t="s">
         <v>55</v>
       </c>
@@ -1317,12 +1649,12 @@
         <v>0.57142899999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="B4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="B5" t="s">
         <v>62</v>
       </c>
@@ -1333,7 +1665,7 @@
         <v>0.57142899999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="B6" t="s">
         <v>63</v>
       </c>
@@ -1344,7 +1676,7 @@
         <v>0.57142899999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="B7" t="s">
         <v>64</v>
       </c>
@@ -1355,7 +1687,7 @@
         <v>0.57142899999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="B8" t="s">
         <v>65</v>
       </c>
@@ -1366,7 +1698,7 @@
         <v>0.57142899999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -1374,7 +1706,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="6" t="s">
         <v>82</v>
       </c>
@@ -1383,7 +1715,7 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12" t="s">
         <v>55</v>
       </c>
@@ -1391,12 +1723,12 @@
         <v>0.53246753000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14" s="7" t="s">
         <v>67</v>
       </c>
@@ -1404,7 +1736,7 @@
         <v>0.61038899999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="B15" s="7" t="s">
         <v>68</v>
       </c>
@@ -1412,7 +1744,7 @@
         <v>0.57142857000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="8" t="s">
         <v>69</v>
       </c>
@@ -1420,7 +1752,7 @@
         <v>0.62337662329999999</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="B17" s="7" t="s">
         <v>66</v>
       </c>
@@ -1428,10 +1760,10 @@
         <v>0.62337662329999999</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="B18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -1442,7 +1774,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="6" t="s">
         <v>82</v>
       </c>
@@ -1451,20 +1783,20 @@
       </c>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="B21" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="28" t="s">
+    <row r="22" spans="1:4">
+      <c r="B22" s="24" t="s">
         <v>66</v>
       </c>
       <c r="C22" s="11">
         <v>0.62337662329999999</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="B23" s="7" t="s">
         <v>67</v>
       </c>
@@ -1472,7 +1804,7 @@
         <v>0.61038899999999996</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="B24" s="7" t="s">
         <v>68</v>
       </c>
@@ -1480,10 +1812,10 @@
         <v>0.57142857000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="15.75" thickBot="1">
       <c r="B25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="12" t="s">
         <v>59</v>
       </c>
@@ -1494,58 +1826,58 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="15"/>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="19">
+      <c r="C28" s="17">
         <v>0.57142857142000003</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
-      <c r="B29" s="21" t="s">
+    <row r="29" spans="1:4">
+      <c r="A29" s="18"/>
+      <c r="B29" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C29" s="22">
+      <c r="C29" s="19">
         <v>0.71298700000000004</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B30" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="27">
+      <c r="C30" s="23">
         <v>0.103896103896103</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="23" t="s">
+    <row r="31" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A31" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="C31" s="25">
+      <c r="C31" s="22">
         <v>0.54545454540000005</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>75</v>
       </c>
@@ -1553,7 +1885,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" s="6" t="s">
         <v>82</v>
       </c>
@@ -1564,7 +1896,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="B35" s="7" t="s">
         <v>77</v>
       </c>
@@ -1572,15 +1904,15 @@
         <v>0.68831168831099998</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="28" t="s">
+    <row r="36" spans="1:3">
+      <c r="B36" s="24" t="s">
         <v>90</v>
       </c>
       <c r="C36" s="11">
         <v>0.70129870129799998</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="B37" s="7" t="s">
         <v>91</v>
       </c>
@@ -1588,7 +1920,7 @@
         <v>0.70129870129799998</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="B38" s="7" t="s">
         <v>78</v>
       </c>
@@ -1596,12 +1928,12 @@
         <v>0.70129870129799998</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="B39" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="B40" s="7" t="s">
         <v>79</v>
       </c>
@@ -1609,7 +1941,7 @@
         <v>0.70129871097999996</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="B41" s="7" t="s">
         <v>80</v>
       </c>
@@ -1617,7 +1949,7 @@
         <v>0.70129871097999996</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>92</v>
       </c>
@@ -1625,7 +1957,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44" s="6" t="s">
         <v>82</v>
       </c>
@@ -1636,7 +1968,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="B45" s="10" t="s">
         <v>93</v>
       </c>
@@ -1644,7 +1976,7 @@
         <v>0.64935064935064901</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="B46" s="10" t="s">
         <v>94</v>
       </c>
@@ -1652,7 +1984,7 @@
         <v>0.662337662337662</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="B47" s="10" t="s">
         <v>95</v>
       </c>
@@ -1660,25 +1992,482 @@
         <v>0.662337662337662</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="28" t="s">
+    <row r="48" spans="1:3">
+      <c r="B48" s="24" t="s">
         <v>80</v>
       </c>
       <c r="C48" s="11">
         <v>0.72727272727299996</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="B49" s="10" t="s">
         <v>95</v>
       </c>
       <c r="C49">
         <v>0.72727272727299996</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>96</v>
+      </c>
+      <c r="B52" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="B53" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F946D1-EBA1-4976-A074-B5CA574C2B51}">
+  <dimension ref="A2:A88"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="97.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1">
+      <c r="A2" s="26" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="25" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="25" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="25" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="27" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="27" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="26" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="25" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="25" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="25" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="25" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="25" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="25" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="25" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="25" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="25" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="25" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="25" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="25" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="25" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="25" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="25" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="25" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="25" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="25" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="25" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="25" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="25" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="25" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="25" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="25" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="25" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="25" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="25" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="25" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="25" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="25" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="25" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="25" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="25" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="25" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="25" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="25" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="25" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="25" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="25" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="25" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="25" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="25" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Layout of Methodology Chapter
</commit_message>
<xml_diff>
--- a/Table of article comparision.xlsx
+++ b/Table of article comparision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c49cb972183112a/Documents OneDrive/06 - CCT Masters in DA/Capstone - 2023/Capstone_Project_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="326" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30AC3093-6150-4297-847D-810B339F3244}"/>
+  <xr:revisionPtr revIDLastSave="329" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80260A3E-5DE7-4B30-8C8F-6772169F617A}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="135" windowWidth="13950" windowHeight="15405" firstSheet="1" activeTab="2" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
+    <workbookView xWindow="14655" yWindow="0" windowWidth="14085" windowHeight="15750" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison Chart" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="183">
   <si>
     <t>Authors</t>
   </si>
@@ -256,16 +256,330 @@
     <t xml:space="preserve">Decision Tree - grouped tenure </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">J48 Decision Tree </t>
-    </r>
+    <t>Algorithm 3</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>Linear</t>
+  </si>
+  <si>
+    <t>sigmoid</t>
+  </si>
+  <si>
+    <t>with GridSearch CV + rbf</t>
+  </si>
+  <si>
+    <t>with GridSearch CV + param_grid</t>
+  </si>
+  <si>
+    <t>with Hyperparm Tuning</t>
+  </si>
+  <si>
+    <t>Target Var</t>
+  </si>
+  <si>
+    <t>Studied Credits</t>
+  </si>
+  <si>
+    <t>studied_credits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decision Tree - Classified  </t>
+  </si>
+  <si>
+    <t>with GridSearchCV</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>Tenure</t>
+  </si>
+  <si>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>rbf (default)</t>
+  </si>
+  <si>
+    <t>poly</t>
+  </si>
+  <si>
+    <t>Algorithm 4</t>
+  </si>
+  <si>
+    <t>Initial Result - 100 trees</t>
+  </si>
+  <si>
+    <t>`@150 trees</t>
+  </si>
+  <si>
+    <t>`@200 trees</t>
+  </si>
+  <si>
+    <t>Algorithm 5</t>
+  </si>
+  <si>
+    <t>MLP - Sequential</t>
+  </si>
+  <si>
+    <t>Epoch 1/10</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 4ms/step - loss: -242081424.0000 - accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 2/10</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 3ms/step - loss: -283053568.0000 - accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 3/10</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 5ms/step - loss: -329420064.0000 - accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 4/10</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 4ms/step - loss: -383456384.0000 - accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 5/10</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 4ms/step - loss: -443147296.0000 - accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 6/10</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 4ms/step - loss: -509580640.0000 - accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 7/10</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 4ms/step - loss: -587204160.0000 - accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 8/10</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 5ms/step - loss: -667973120.0000 - accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 9/10</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 4ms/step - loss: -764345728.0000 - accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 10/10</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 4ms/step - loss: -866226176.0000 - accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test 2 </t>
+  </si>
+  <si>
+    <t>Initial Test - 2 hidden layers  with relu and sigmoid as the activation layer</t>
+  </si>
+  <si>
+    <t>Studiet Credits as dependant layer .. Loss function = binary_crossentropy and optimizer = adam</t>
+  </si>
+  <si>
+    <t>Epoch 1/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 13ms/step - loss: -25394743296.0000 - accuracy: 0.0000e+00 - val_loss: -24771162112.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 2/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 8ms/step - loss: -26108925952.0000 - accuracy: 0.0000e+00 - val_loss: -25442850816.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 3/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 8ms/step - loss: -26816679936.0000 - accuracy: 0.0000e+00 - val_loss: -26138527744.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 4/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 9ms/step - loss: -27543879680.0000 - accuracy: 0.0000e+00 - val_loss: -26850807808.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 5/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 8ms/step - loss: -28280655872.0000 - accuracy: 0.0000e+00 - val_loss: -27573581824.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 6/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 8ms/step - loss: -29059145728.0000 - accuracy: 0.0000e+00 - val_loss: -28300064768.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 7/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 8ms/step - loss: -29805772800.0000 - accuracy: 0.0000e+00 - val_loss: -29048614912.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 8/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 8ms/step - loss: -30605600768.0000 - accuracy: 0.0000e+00 - val_loss: -29793935360.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 9/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 8ms/step - loss: -31385100288.0000 - accuracy: 0.0000e+00 - val_loss: -30564853760.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 10/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 8ms/step - loss: -32193349632.0000 - accuracy: 0.0000e+00 - val_loss: -31354171392.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 11/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 11ms/step - loss: -33020014592.0000 - accuracy: 0.0000e+00 - val_loss: -32140675072.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 12/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 9ms/step - loss: -33841115136.0000 - accuracy: 0.0000e+00 - val_loss: -32941174784.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 13/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 12ms/step - loss: -34674659328.0000 - accuracy: 0.0000e+00 - val_loss: -33758574592.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 14/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 8ms/step - loss: -35518062592.0000 - accuracy: 0.0000e+00 - val_loss: -34595278848.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 15/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 9ms/step - loss: -36400070656.0000 - accuracy: 0.0000e+00 - val_loss: -35426832384.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 16/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 9ms/step - loss: -37296611328.0000 - accuracy: 0.0000e+00 - val_loss: -36265394176.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 17/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 10ms/step - loss: -38146936832.0000 - accuracy: 0.0000e+00 - val_loss: -37156323328.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 18/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 9ms/step - loss: -39079579648.0000 - accuracy: 0.0000e+00 - val_loss: -38033629184.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 19/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 8ms/step - loss: -39998951424.0000 - accuracy: 0.0000e+00 - val_loss: -38920065024.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 20/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 9ms/step - loss: -40929095680.0000 - accuracy: 0.0000e+00 - val_loss: -39829299200.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 21/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 9ms/step - loss: -41876824064.0000 - accuracy: 0.0000e+00 - val_loss: -40747204608.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 22/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 9ms/step - loss: -42839941120.0000 - accuracy: 0.0000e+00 - val_loss: -41662656512.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 23/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 8ms/step - loss: -43813273600.0000 - accuracy: 0.0000e+00 - val_loss: -42587631616.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 24/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 9ms/step - loss: -44752834560.0000 - accuracy: 0.0000e+00 - val_loss: -43560857600.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 25/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 9ms/step - loss: -45789294592.0000 - accuracy: 0.0000e+00 - val_loss: -44508856320.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 26/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 10ms/step - loss: -46798168064.0000 - accuracy: 0.0000e+00 - val_loss: -45485510656.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 27/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 10ms/step - loss: -47796768768.0000 - accuracy: 0.0000e+00 - val_loss: -46478618624.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 28/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 10ms/step - loss: -48838012928.0000 - accuracy: 0.0000e+00 - val_loss: -47475539968.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 29/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 9ms/step - loss: -49879625728.0000 - accuracy: 0.0000e+00 - val_loss: -48487399424.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>Epoch 30/30</t>
+  </si>
+  <si>
+    <t>10/10 [==============================] - 0s 8ms/step - loss: -50940579840.0000 - accuracy: 0.0000e+00 - val_loss: -49510993920.0000 - val_accuracy: 0.0000e+00</t>
+  </si>
+  <si>
+    <t>2 hidden Layers with relu and sigmoid as the final activation layer</t>
+  </si>
+  <si>
+    <t>Student ID as dependant layer .. Loss function = binary_crossentropy and optimizer = adam</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -274,20 +588,10 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">/ JRIP / Gradient-boosted Classifiers </t>
+      <t>Logistic Regression + 10-Fold Validation</t>
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">5-fold cross validation </t>
-    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -296,20 +600,10 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>+SVC rbf algorithm</t>
+      <t xml:space="preserve">J48 Decision Tree / JRIP / Gradient-boosted Classifiers </t>
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Logistic Regression</t>
-    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -318,345 +612,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> + </t>
+      <t>5-fold cross validation +SVC rbf algorithm</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>10-Fold Validation</t>
-    </r>
-  </si>
-  <si>
-    <t>Algorithm 3</t>
-  </si>
-  <si>
-    <t>SVM</t>
-  </si>
-  <si>
-    <t>Linear</t>
-  </si>
-  <si>
-    <t>sigmoid</t>
-  </si>
-  <si>
-    <t>with GridSearch CV + rbf</t>
-  </si>
-  <si>
-    <t>with GridSearch CV + param_grid</t>
-  </si>
-  <si>
-    <t>with Hyperparm Tuning</t>
-  </si>
-  <si>
-    <t>Target Var</t>
-  </si>
-  <si>
-    <t>Studied Credits</t>
-  </si>
-  <si>
-    <t>studied_credits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decision Tree - Classified  </t>
-  </si>
-  <si>
-    <t>with GridSearchCV</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>Tenure</t>
-  </si>
-  <si>
-    <t>Random Forest</t>
-  </si>
-  <si>
-    <t>rbf (default)</t>
-  </si>
-  <si>
-    <t>poly</t>
-  </si>
-  <si>
-    <t>Algorithm 4</t>
-  </si>
-  <si>
-    <t>Initial Result - 100 trees</t>
-  </si>
-  <si>
-    <t>`@150 trees</t>
-  </si>
-  <si>
-    <t>`@200 trees</t>
-  </si>
-  <si>
-    <t>Algorithm 5</t>
-  </si>
-  <si>
-    <t>MLP - Sequential</t>
-  </si>
-  <si>
-    <t>Epoch 1/10</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 4ms/step - loss: -242081424.0000 - accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 2/10</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 3ms/step - loss: -283053568.0000 - accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 3/10</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 5ms/step - loss: -329420064.0000 - accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 4/10</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 4ms/step - loss: -383456384.0000 - accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 5/10</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 4ms/step - loss: -443147296.0000 - accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 6/10</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 4ms/step - loss: -509580640.0000 - accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 7/10</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 4ms/step - loss: -587204160.0000 - accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 8/10</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 5ms/step - loss: -667973120.0000 - accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 9/10</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 4ms/step - loss: -764345728.0000 - accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 10/10</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 4ms/step - loss: -866226176.0000 - accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initial Test - 2 hidden layers </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test 2 </t>
-  </si>
-  <si>
-    <t>Initial Test - 2 hidden layers  with relu and sigmoid as the activation layer</t>
-  </si>
-  <si>
-    <t>Studiet Credits as dependant layer .. Loss function = binary_crossentropy and optimizer = adam</t>
-  </si>
-  <si>
-    <t>Epoch 1/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 13ms/step - loss: -25394743296.0000 - accuracy: 0.0000e+00 - val_loss: -24771162112.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 2/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 8ms/step - loss: -26108925952.0000 - accuracy: 0.0000e+00 - val_loss: -25442850816.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 3/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 8ms/step - loss: -26816679936.0000 - accuracy: 0.0000e+00 - val_loss: -26138527744.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 4/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 9ms/step - loss: -27543879680.0000 - accuracy: 0.0000e+00 - val_loss: -26850807808.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 5/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 8ms/step - loss: -28280655872.0000 - accuracy: 0.0000e+00 - val_loss: -27573581824.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 6/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 8ms/step - loss: -29059145728.0000 - accuracy: 0.0000e+00 - val_loss: -28300064768.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 7/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 8ms/step - loss: -29805772800.0000 - accuracy: 0.0000e+00 - val_loss: -29048614912.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 8/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 8ms/step - loss: -30605600768.0000 - accuracy: 0.0000e+00 - val_loss: -29793935360.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 9/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 8ms/step - loss: -31385100288.0000 - accuracy: 0.0000e+00 - val_loss: -30564853760.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 10/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 8ms/step - loss: -32193349632.0000 - accuracy: 0.0000e+00 - val_loss: -31354171392.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 11/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 11ms/step - loss: -33020014592.0000 - accuracy: 0.0000e+00 - val_loss: -32140675072.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 12/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 9ms/step - loss: -33841115136.0000 - accuracy: 0.0000e+00 - val_loss: -32941174784.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 13/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 12ms/step - loss: -34674659328.0000 - accuracy: 0.0000e+00 - val_loss: -33758574592.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 14/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 8ms/step - loss: -35518062592.0000 - accuracy: 0.0000e+00 - val_loss: -34595278848.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 15/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 9ms/step - loss: -36400070656.0000 - accuracy: 0.0000e+00 - val_loss: -35426832384.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 16/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 9ms/step - loss: -37296611328.0000 - accuracy: 0.0000e+00 - val_loss: -36265394176.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 17/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 10ms/step - loss: -38146936832.0000 - accuracy: 0.0000e+00 - val_loss: -37156323328.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 18/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 9ms/step - loss: -39079579648.0000 - accuracy: 0.0000e+00 - val_loss: -38033629184.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 19/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 8ms/step - loss: -39998951424.0000 - accuracy: 0.0000e+00 - val_loss: -38920065024.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 20/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 9ms/step - loss: -40929095680.0000 - accuracy: 0.0000e+00 - val_loss: -39829299200.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 21/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 9ms/step - loss: -41876824064.0000 - accuracy: 0.0000e+00 - val_loss: -40747204608.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 22/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 9ms/step - loss: -42839941120.0000 - accuracy: 0.0000e+00 - val_loss: -41662656512.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 23/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 8ms/step - loss: -43813273600.0000 - accuracy: 0.0000e+00 - val_loss: -42587631616.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 24/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 9ms/step - loss: -44752834560.0000 - accuracy: 0.0000e+00 - val_loss: -43560857600.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 25/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 9ms/step - loss: -45789294592.0000 - accuracy: 0.0000e+00 - val_loss: -44508856320.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 26/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 10ms/step - loss: -46798168064.0000 - accuracy: 0.0000e+00 - val_loss: -45485510656.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 27/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 10ms/step - loss: -47796768768.0000 - accuracy: 0.0000e+00 - val_loss: -46478618624.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 28/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 10ms/step - loss: -48838012928.0000 - accuracy: 0.0000e+00 - val_loss: -47475539968.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 29/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 9ms/step - loss: -49879625728.0000 - accuracy: 0.0000e+00 - val_loss: -48487399424.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>Epoch 30/30</t>
-  </si>
-  <si>
-    <t>10/10 [==============================] - 0s 8ms/step - loss: -50940579840.0000 - accuracy: 0.0000e+00 - val_loss: -49510993920.0000 - val_accuracy: 0.0000e+00</t>
-  </si>
-  <si>
-    <t>2 hidden Layers with relu and sigmoid as the final activation layer</t>
-  </si>
-  <si>
-    <t>Student ID as dependant layer .. Loss function = binary_crossentropy and optimizer = adam</t>
   </si>
 </sst>
 </file>
@@ -666,7 +623,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -705,6 +662,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -819,7 +783,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -869,6 +833,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1244,7 +1211,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" sqref="A1:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1254,7 +1221,7 @@
     <col min="3" max="3" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="30.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="6" max="6" width="0" style="2" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="25.42578125" style="2" customWidth="1"/>
     <col min="8" max="8" width="19.42578125" style="2" customWidth="1"/>
     <col min="9" max="9" width="24.85546875" style="2" customWidth="1"/>
@@ -1320,8 +1287,8 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>74</v>
+      <c r="E3" s="28" t="s">
+        <v>180</v>
       </c>
       <c r="F3" s="4">
         <v>0.80700000000000005</v>
@@ -1343,8 +1310,8 @@
       <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>72</v>
+      <c r="E4" s="28" t="s">
+        <v>181</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>18</v>
@@ -1359,7 +1326,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30">
+    <row r="5" spans="1:9">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1372,7 +1339,7 @@
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="28" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="3">
@@ -1395,7 +1362,7 @@
       <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="28" t="s">
         <v>25</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -1418,8 +1385,8 @@
       <c r="D7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>73</v>
+      <c r="E7" s="28" t="s">
+        <v>182</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>28</v>
@@ -1438,7 +1405,7 @@
       <c r="D8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="28" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1455,7 +1422,7 @@
       <c r="D9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="28" t="s">
         <v>35</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -1605,10 +1572,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61403218-7A3E-4B26-8B7C-D3F4D407424F}">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1629,7 +1596,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>57</v>
@@ -1708,7 +1675,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>60</v>
@@ -1771,12 +1738,12 @@
         <v>70</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>60</v>
@@ -1820,18 +1787,18 @@
         <v>59</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>60</v>
@@ -1849,7 +1816,7 @@
     <row r="29" spans="1:4">
       <c r="A29" s="18"/>
       <c r="B29" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C29" s="19">
         <v>0.71298700000000004</v>
@@ -1857,10 +1824,10 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C30" s="23">
         <v>0.103896103896103</v>
@@ -1868,10 +1835,10 @@
     </row>
     <row r="31" spans="1:4" ht="15.75" thickBot="1">
       <c r="A31" s="20" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C31" s="22">
         <v>0.54545454540000005</v>
@@ -1879,18 +1846,18 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B33" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>60</v>
@@ -1898,7 +1865,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="B35" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C35">
         <v>0.68831168831099998</v>
@@ -1906,7 +1873,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="B36" s="24" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C36" s="11">
         <v>0.70129870129799998</v>
@@ -1914,7 +1881,7 @@
     </row>
     <row r="37" spans="1:3">
       <c r="B37" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C37">
         <v>0.70129870129799998</v>
@@ -1922,7 +1889,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="B38" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C38">
         <v>0.70129870129799998</v>
@@ -1930,12 +1897,12 @@
     </row>
     <row r="39" spans="1:3">
       <c r="B39" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="B40" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C40">
         <v>0.70129871097999996</v>
@@ -1943,7 +1910,7 @@
     </row>
     <row r="41" spans="1:3">
       <c r="B41" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C41">
         <v>0.70129871097999996</v>
@@ -1951,18 +1918,18 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B43" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B44" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>60</v>
@@ -1970,7 +1937,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="B45" s="10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C45">
         <v>0.64935064935064901</v>
@@ -1978,7 +1945,7 @@
     </row>
     <row r="46" spans="1:3">
       <c r="B46" s="10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C46">
         <v>0.662337662337662</v>
@@ -1986,7 +1953,7 @@
     </row>
     <row r="47" spans="1:3">
       <c r="B47" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C47">
         <v>0.662337662337662</v>
@@ -1994,7 +1961,7 @@
     </row>
     <row r="48" spans="1:3">
       <c r="B48" s="24" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C48" s="11">
         <v>0.72727272727299996</v>
@@ -2002,7 +1969,7 @@
     </row>
     <row r="49" spans="1:3">
       <c r="B49" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C49">
         <v>0.72727272727299996</v>
@@ -2010,15 +1977,10 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B52" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="B53" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2033,7 +1995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F946D1-EBA1-4976-A074-B5CA574C2B51}">
   <dimension ref="A2:A88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
@@ -2044,427 +2006,427 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" s="26" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="26" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="25" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="25" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="25" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="25" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="25" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="25" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="25" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="25" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="25" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="25" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="25" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="25" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="25" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="25" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="25" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="25" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="25" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="25" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="27" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="27" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="26" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="25" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="25" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="25" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="25" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="25" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="25" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="25" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="25" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="25" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="25" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="25" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="25" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="25" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="25" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="25" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="25" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="25" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="25" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="25" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="25" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="25" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="25" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="25" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="25" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="25" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="25" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="25" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="25" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="25" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="25" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="25" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" s="25" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="25" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="25" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" s="25" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="25" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="25" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="25" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="25" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="25" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="25" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="25" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="25" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="25" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="25" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" s="25" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" s="25" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="25" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="25" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="25" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" s="25" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" s="25" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="25" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="25" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" s="25" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" s="25" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" s="25" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" s="25" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" s="25" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="25" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Methodolgy - work on justifying selected algorithms 1 to 3
</commit_message>
<xml_diff>
--- a/Table of article comparision.xlsx
+++ b/Table of article comparision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c49cb972183112a/Documents OneDrive/06 - CCT Masters in DA/Capstone - 2023/Capstone_Project_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="329" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80260A3E-5DE7-4B30-8C8F-6772169F617A}"/>
+  <xr:revisionPtr revIDLastSave="331" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{790AB53B-7717-4064-95D6-651AD02D74E7}"/>
   <bookViews>
-    <workbookView xWindow="14655" yWindow="0" windowWidth="14085" windowHeight="15750" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
+    <workbookView xWindow="44370" yWindow="1305" windowWidth="13140" windowHeight="14400" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison Chart" sheetId="1" r:id="rId1"/>
@@ -623,7 +623,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -662,13 +662,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -783,7 +776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -834,9 +827,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -865,7 +855,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>546984</xdr:colOff>
+      <xdr:colOff>237422</xdr:colOff>
       <xdr:row>70</xdr:row>
       <xdr:rowOff>190061</xdr:rowOff>
     </xdr:to>
@@ -901,10 +891,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1287,7 +1273,7 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="2" t="s">
         <v>180</v>
       </c>
       <c r="F3" s="4">
@@ -1310,7 +1296,7 @@
       <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="2" t="s">
         <v>181</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -1339,7 +1325,7 @@
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="3">
@@ -1362,7 +1348,7 @@
       <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -1385,7 +1371,7 @@
       <c r="D7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="2" t="s">
         <v>182</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -1405,7 +1391,7 @@
       <c r="D8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1422,7 +1408,7 @@
       <c r="D9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="2" t="s">
         <v>35</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -1574,14 +1560,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61403218-7A3E-4B26-8B7C-D3F4D407424F}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Completion of Methodology Chapter and start on Implementation
plus update to notebooks
</commit_message>
<xml_diff>
--- a/Table of article comparision.xlsx
+++ b/Table of article comparision.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c49cb972183112a/Documents OneDrive/06 - CCT Masters in DA/Capstone - 2023/Capstone_Project_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="331" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{790AB53B-7717-4064-95D6-651AD02D74E7}"/>
+  <xr:revisionPtr revIDLastSave="407" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBDDA001-BB5B-47A1-B768-C7E150708823}"/>
   <bookViews>
-    <workbookView xWindow="44370" yWindow="1305" windowWidth="13140" windowHeight="14400" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
+    <workbookView xWindow="42360" yWindow="420" windowWidth="13140" windowHeight="14400" firstSheet="1" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison Chart" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="191">
   <si>
     <t>Authors</t>
   </si>
@@ -614,6 +614,30 @@
       </rPr>
       <t>5-fold cross validation +SVC rbf algorithm</t>
     </r>
+  </si>
+  <si>
+    <t>criterion='entropy'</t>
+  </si>
+  <si>
+    <t>criterion='gini'</t>
+  </si>
+  <si>
+    <t>32 neurons + 16</t>
+  </si>
+  <si>
+    <t>Test 2</t>
+  </si>
+  <si>
+    <t>20 neurons + 10</t>
+  </si>
+  <si>
+    <t>Test 3</t>
+  </si>
+  <si>
+    <t>Test 1</t>
+  </si>
+  <si>
+    <t>50 neurons + 20</t>
   </si>
 </sst>
 </file>
@@ -776,7 +800,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -827,6 +851,9 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -849,15 +876,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>466726</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>192882</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>21443</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>237422</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>190061</xdr:rowOff>
+      <xdr:colOff>261936</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>178155</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -880,8 +907,140 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="466726" y="10353675"/>
-          <a:ext cx="5395208" cy="3190436"/>
+          <a:off x="192882" y="11475256"/>
+          <a:ext cx="5736429" cy="3395212"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>273844</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2178493</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>109087</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E14219AB-C609-E9B4-B241-A343F1F6A8C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="273844" y="15573376"/>
+          <a:ext cx="2809524" cy="3609524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>640192</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>113833</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4266CCAD-E7E9-D3E7-62FB-23681E5FC361}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3643313" y="15644813"/>
+          <a:ext cx="2914286" cy="3733333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>27964</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>75762</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14E2D63C-F537-910B-B92B-A8ECB52E7A32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7298531" y="15454313"/>
+          <a:ext cx="4885714" cy="3504762"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -891,6 +1050,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1558,21 +1721,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61403218-7A3E-4B26-8B7C-D3F4D407424F}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -1580,7 +1746,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
         <v>79</v>
       </c>
@@ -1591,7 +1757,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:7">
       <c r="B3" t="s">
         <v>55</v>
       </c>
@@ -1602,12 +1768,12 @@
         <v>0.57142899999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:7">
       <c r="B4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:7">
       <c r="B5" t="s">
         <v>62</v>
       </c>
@@ -1618,7 +1784,7 @@
         <v>0.57142899999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="B6" t="s">
         <v>63</v>
       </c>
@@ -1629,7 +1795,7 @@
         <v>0.57142899999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="B7" t="s">
         <v>64</v>
       </c>
@@ -1640,7 +1806,7 @@
         <v>0.57142899999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="B8" t="s">
         <v>65</v>
       </c>
@@ -1651,15 +1817,16 @@
         <v>0.57142899999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>59</v>
       </c>
       <c r="B10" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="6" t="s">
         <v>79</v>
       </c>
@@ -1667,8 +1834,10 @@
         <v>60</v>
       </c>
       <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" s="6"/>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:7">
       <c r="B12" t="s">
         <v>55</v>
       </c>
@@ -1676,28 +1845,32 @@
         <v>0.53246753000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:7">
       <c r="B13" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="F13" s="24"/>
+      <c r="G13" s="11"/>
+    </row>
+    <row r="14" spans="1:7">
       <c r="B14" s="7" t="s">
         <v>67</v>
       </c>
       <c r="C14">
         <v>0.61038899999999996</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:7">
       <c r="B15" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C15">
         <v>0.57142857000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:7">
       <c r="B16" s="8" t="s">
         <v>69</v>
       </c>
@@ -1775,9 +1948,7 @@
       <c r="B26" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="14" t="s">
-        <v>79</v>
-      </c>
+      <c r="C26" s="14"/>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="15" t="s">
@@ -1922,6 +2093,9 @@
       </c>
     </row>
     <row r="45" spans="1:3">
+      <c r="A45" s="28" t="s">
+        <v>183</v>
+      </c>
       <c r="B45" s="10" t="s">
         <v>90</v>
       </c>
@@ -1930,6 +2104,7 @@
       </c>
     </row>
     <row r="46" spans="1:3">
+      <c r="A46" s="28"/>
       <c r="B46" s="10" t="s">
         <v>91</v>
       </c>
@@ -1938,6 +2113,7 @@
       </c>
     </row>
     <row r="47" spans="1:3">
+      <c r="A47" s="28"/>
       <c r="B47" s="10" t="s">
         <v>92</v>
       </c>
@@ -1946,6 +2122,7 @@
       </c>
     </row>
     <row r="48" spans="1:3">
+      <c r="A48" s="28"/>
       <c r="B48" s="24" t="s">
         <v>77</v>
       </c>
@@ -1954,6 +2131,7 @@
       </c>
     </row>
     <row r="49" spans="1:3">
+      <c r="A49" s="28"/>
       <c r="B49" s="10" t="s">
         <v>92</v>
       </c>
@@ -1961,15 +2139,89 @@
         <v>0.72727272727299996</v>
       </c>
     </row>
+    <row r="50" spans="1:3">
+      <c r="B50" s="10"/>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51">
+        <v>0.64935064935064901</v>
+      </c>
+    </row>
     <row r="52" spans="1:3">
-      <c r="A52" t="s">
+      <c r="A52" s="28"/>
+      <c r="B52" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C52" s="11">
+        <v>0.68831168831168799</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="10"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="10"/>
+      <c r="B54" s="10"/>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="B55" s="10"/>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
         <v>93</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B56" t="s">
         <v>94</v>
       </c>
     </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="B57" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="B58" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B59" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" t="s">
+        <v>189</v>
+      </c>
+      <c r="C81" t="s">
+        <v>186</v>
+      </c>
+      <c r="G81" t="s">
+        <v>188</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="A51:A52"/>
+  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Results & Implement - Algorithm 4
</commit_message>
<xml_diff>
--- a/Table of article comparision.xlsx
+++ b/Table of article comparision.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c49cb972183112a/Documents OneDrive/06 - CCT Masters in DA/Capstone - 2023/Capstone_Project_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="407" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBDDA001-BB5B-47A1-B768-C7E150708823}"/>
+  <xr:revisionPtr revIDLastSave="410" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C23639EC-4550-4ED7-88E5-B936069B400E}"/>
   <bookViews>
     <workbookView xWindow="42360" yWindow="420" windowWidth="13140" windowHeight="14400" firstSheet="1" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
   </bookViews>
@@ -881,8 +881,8 @@
       <xdr:rowOff>21443</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>261936</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>702467</xdr:colOff>
       <xdr:row>77</xdr:row>
       <xdr:rowOff>178155</xdr:rowOff>
     </xdr:to>
@@ -926,7 +926,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2178493</xdr:colOff>
+      <xdr:colOff>1797493</xdr:colOff>
       <xdr:row>100</xdr:row>
       <xdr:rowOff>109087</xdr:rowOff>
     </xdr:to>
@@ -1723,13 +1723,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61403218-7A3E-4B26-8B7C-D3F4D407424F}">
   <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:C31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.28515625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="6.7109375" customWidth="1"/>

</xml_diff>

<commit_message>
Results & Implementation - Algorithms 4 & 5
</commit_message>
<xml_diff>
--- a/Table of article comparision.xlsx
+++ b/Table of article comparision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c49cb972183112a/Documents OneDrive/06 - CCT Masters in DA/Capstone - 2023/Capstone_Project_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="410" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C23639EC-4550-4ED7-88E5-B936069B400E}"/>
+  <xr:revisionPtr revIDLastSave="456" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FD1B888-17D1-4601-99C1-AE5910B65668}"/>
   <bookViews>
-    <workbookView xWindow="42360" yWindow="420" windowWidth="13140" windowHeight="14400" firstSheet="1" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="1" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison Chart" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="198">
   <si>
     <t>Authors</t>
   </si>
@@ -639,6 +639,27 @@
   <si>
     <t>50 neurons + 20</t>
   </si>
+  <si>
+    <t>32 neurons + 16 with Hyperparmameter Tuning</t>
+  </si>
+  <si>
+    <t>Algorithm 1 - Logistic Regression</t>
+  </si>
+  <si>
+    <t>Algorithm 2 - Decision Tree</t>
+  </si>
+  <si>
+    <t>Algorithm 3 - Support Vector Machines (SVM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Algorithm 4 - Random Forest </t>
+  </si>
+  <si>
+    <t>Algorithm5 - Multi-Layer Perceptron (MLP)</t>
+  </si>
+  <si>
+    <t>Accuracy Result</t>
+  </si>
 </sst>
 </file>
 
@@ -647,7 +668,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -687,6 +708,13 @@
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -708,7 +736,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -796,11 +824,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -854,9 +898,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -877,13 +930,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>192882</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>21443</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>702467</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:colOff>11905</xdr:colOff>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>178155</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -921,13 +974,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>273844</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>119063</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1797493</xdr:colOff>
-      <xdr:row>100</xdr:row>
+      <xdr:row>101</xdr:row>
       <xdr:rowOff>109087</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -965,13 +1018,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>640192</xdr:colOff>
-      <xdr:row>101</xdr:row>
+      <xdr:row>102</xdr:row>
       <xdr:rowOff>113833</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1009,13 +1062,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>27964</xdr:colOff>
-      <xdr:row>99</xdr:row>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>623277</xdr:colOff>
+      <xdr:row>100</xdr:row>
       <xdr:rowOff>75762</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1721,24 +1774,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61403218-7A3E-4B26-8B7C-D3F4D407424F}">
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:C52"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.28515625" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="6.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.42578125" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -1746,7 +1801,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:11">
       <c r="A2" s="6" t="s">
         <v>79</v>
       </c>
@@ -1757,7 +1812,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:11">
       <c r="B3" t="s">
         <v>55</v>
       </c>
@@ -1768,12 +1823,12 @@
         <v>0.57142899999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:11">
       <c r="B4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:11">
       <c r="B5" t="s">
         <v>62</v>
       </c>
@@ -1784,7 +1839,7 @@
         <v>0.57142899999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:11">
       <c r="B6" t="s">
         <v>63</v>
       </c>
@@ -1795,7 +1850,7 @@
         <v>0.57142899999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:11">
       <c r="B7" t="s">
         <v>64</v>
       </c>
@@ -1805,8 +1860,12 @@
       <c r="D7">
         <v>0.57142899999999996</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="J7" s="30"/>
+      <c r="K7" s="31" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="B8" t="s">
         <v>65</v>
       </c>
@@ -1816,8 +1875,22 @@
       <c r="D8">
         <v>0.57142899999999996</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="J8" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="K8" s="32">
+        <v>0.62091499999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="J9" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="K9" s="32">
+        <v>0.71298700000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -1825,8 +1898,14 @@
         <v>71</v>
       </c>
       <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="J10" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="K10" s="32">
+        <v>0.70129870129799998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="6" t="s">
         <v>79</v>
       </c>
@@ -1836,41 +1915,50 @@
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="J11" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="K11" s="32">
+        <v>0.72727272727299996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="B12" t="s">
         <v>55</v>
       </c>
       <c r="C12">
         <v>0.53246753000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="J12" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="K12" s="32">
+        <v>0.66993499999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="B13" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="11"/>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:11">
       <c r="B14" s="7" t="s">
         <v>67</v>
       </c>
       <c r="C14">
         <v>0.61038899999999996</v>
       </c>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:7">
+    </row>
+    <row r="15" spans="1:11">
       <c r="B15" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C15">
         <v>0.57142857000000002</v>
       </c>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:7">
+    </row>
+    <row r="16" spans="1:11">
       <c r="B16" s="8" t="s">
         <v>69</v>
       </c>
@@ -2126,9 +2214,7 @@
       <c r="B48" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="C48" s="11">
-        <v>0.72727272727299996</v>
-      </c>
+      <c r="C48" s="11"/>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="28"/>
@@ -2158,14 +2244,16 @@
       <c r="B52" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="C52" s="11">
+      <c r="C52" s="11"/>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="28"/>
+      <c r="B53" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53" s="29">
         <v>0.68831168831168799</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="10"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="10"/>
@@ -2199,28 +2287,34 @@
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="10" t="s">
+      <c r="A59" s="10"/>
+      <c r="B59" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
-      <c r="A81" t="s">
+    <row r="82" spans="1:7">
+      <c r="A82" t="s">
         <v>189</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C82" t="s">
         <v>186</v>
       </c>
-      <c r="G81" t="s">
+      <c r="G82" t="s">
         <v>188</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A45:A49"/>
-    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A51:A53"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Work on applying the variables for the result section to model 1 and 2
</commit_message>
<xml_diff>
--- a/Table of article comparision.xlsx
+++ b/Table of article comparision.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c49cb972183112a/Documents OneDrive/06 - CCT Masters in DA/Capstone - 2023/Capstone_Project_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="456" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FD1B888-17D1-4601-99C1-AE5910B65668}"/>
+  <xr:revisionPtr revIDLastSave="483" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9C1EFD6-1CDF-483F-A118-1ACAD9591E8B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="1" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="201">
   <si>
     <t>Authors</t>
   </si>
@@ -284,9 +284,6 @@
   </si>
   <si>
     <t>studied_credits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decision Tree - Classified  </t>
   </si>
   <si>
     <t>with GridSearchCV</t>
@@ -659,6 +656,18 @@
   </si>
   <si>
     <t>Accuracy Result</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Studied_Credits</t>
+  </si>
+  <si>
+    <t>Accuracy result by variable for each modle</t>
+  </si>
+  <si>
+    <t>Decision Tree - categorical data</t>
   </si>
 </sst>
 </file>
@@ -736,7 +745,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -839,12 +848,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -895,15 +941,38 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1490,7 +1559,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F3" s="4">
         <v>0.80700000000000005</v>
@@ -1513,7 +1582,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>18</v>
@@ -1588,7 +1657,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>28</v>
@@ -1774,10 +1843,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61403218-7A3E-4B26-8B7C-D3F4D407424F}">
-  <dimension ref="A1:K82"/>
+  <dimension ref="A1:M82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:K12"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1791,9 +1860,11 @@
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="45.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -1801,10 +1872,13 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:13">
       <c r="A2" s="6" t="s">
         <v>79</v>
       </c>
+      <c r="B2" t="s">
+        <v>197</v>
+      </c>
       <c r="C2" s="6" t="s">
         <v>57</v>
       </c>
@@ -1812,7 +1886,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:13">
       <c r="B3" t="s">
         <v>55</v>
       </c>
@@ -1823,12 +1897,12 @@
         <v>0.57142899999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:13">
       <c r="B4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:13">
       <c r="B5" t="s">
         <v>62</v>
       </c>
@@ -1839,7 +1913,7 @@
         <v>0.57142899999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:13">
       <c r="B6" t="s">
         <v>63</v>
       </c>
@@ -1850,7 +1924,7 @@
         <v>0.57142899999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:13">
       <c r="B7" t="s">
         <v>64</v>
       </c>
@@ -1860,12 +1934,12 @@
       <c r="D7">
         <v>0.57142899999999996</v>
       </c>
-      <c r="J7" s="30"/>
-      <c r="K7" s="31" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="J7" s="28"/>
+      <c r="K7" s="29" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="B8" t="s">
         <v>65</v>
       </c>
@@ -1875,22 +1949,22 @@
       <c r="D8">
         <v>0.57142899999999996</v>
       </c>
-      <c r="J8" s="30" t="s">
+      <c r="J8" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="K8" s="30">
+        <v>0.62091499999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="J9" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="K8" s="32">
-        <v>0.62091499999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="J9" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="K9" s="32">
+      <c r="K9" s="30">
         <v>0.71298700000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -1898,14 +1972,14 @@
         <v>71</v>
       </c>
       <c r="G10" s="6"/>
-      <c r="J10" s="30" t="s">
-        <v>194</v>
-      </c>
-      <c r="K10" s="32">
+      <c r="J10" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="K10" s="30">
         <v>0.70129870129799998</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:13">
       <c r="A11" s="6" t="s">
         <v>79</v>
       </c>
@@ -1915,34 +1989,34 @@
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="G11" s="6"/>
-      <c r="J11" s="30" t="s">
-        <v>195</v>
-      </c>
-      <c r="K11" s="32">
+      <c r="J11" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="K11" s="30">
         <v>0.72727272727299996</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:13">
       <c r="B12" t="s">
         <v>55</v>
       </c>
       <c r="C12">
         <v>0.53246753000000002</v>
       </c>
-      <c r="J12" s="30" t="s">
-        <v>196</v>
-      </c>
-      <c r="K12" s="32">
+      <c r="J12" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="K12" s="30">
         <v>0.66993499999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:13">
       <c r="B13" t="s">
         <v>61</v>
       </c>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:13">
       <c r="B14" s="7" t="s">
         <v>67</v>
       </c>
@@ -1950,34 +2024,69 @@
         <v>0.61038899999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:13">
       <c r="B15" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C15">
         <v>0.57142857000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="K15" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="L15" s="33"/>
+      <c r="M15" s="34"/>
+    </row>
+    <row r="16" spans="1:13">
       <c r="B16" s="8" t="s">
         <v>69</v>
       </c>
       <c r="C16" s="9">
         <v>0.62337662329999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="J16" s="28"/>
+      <c r="K16" s="36" t="s">
+        <v>197</v>
+      </c>
+      <c r="L16" s="36" t="s">
+        <v>198</v>
+      </c>
+      <c r="M16" s="36" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="B17" s="7" t="s">
         <v>66</v>
       </c>
       <c r="C17">
         <v>0.62337662329999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="J17" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="K17" s="38">
+        <v>0.62090000000000001</v>
+      </c>
+      <c r="L17" s="39">
+        <v>0.66990000000000005</v>
+      </c>
+      <c r="M17" s="37">
+        <v>7.5200000000000003E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="B18" s="7"/>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="J18" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="K18" s="35">
+        <v>0.51948051948051899</v>
+      </c>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -1987,8 +2096,14 @@
       <c r="C19" s="6" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="J19" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="K19" s="35"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="6" t="s">
         <v>79</v>
       </c>
@@ -1996,13 +2111,25 @@
         <v>60</v>
       </c>
       <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="J20" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="K20" s="35"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
+    </row>
+    <row r="21" spans="1:13">
       <c r="B21" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="J21" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="K21" s="35"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+    </row>
+    <row r="22" spans="1:13">
       <c r="B22" s="24" t="s">
         <v>66</v>
       </c>
@@ -2010,7 +2137,7 @@
         <v>0.62337662329999999</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:13">
       <c r="B23" s="7" t="s">
         <v>67</v>
       </c>
@@ -2018,7 +2145,7 @@
         <v>0.61038899999999996</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:13">
       <c r="B24" s="7" t="s">
         <v>68</v>
       </c>
@@ -2026,19 +2153,19 @@
         <v>0.57142857000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" thickBot="1">
+    <row r="25" spans="1:13" ht="15.75" thickBot="1">
       <c r="B25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:13">
       <c r="A26" s="12" t="s">
         <v>59</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>82</v>
+        <v>200</v>
       </c>
       <c r="C26" s="14"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:13">
       <c r="A27" s="15" t="s">
         <v>79</v>
       </c>
@@ -2049,7 +2176,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:13">
       <c r="A28" s="15"/>
       <c r="B28" s="10" t="s">
         <v>55</v>
@@ -2058,32 +2185,32 @@
         <v>0.57142857142000003</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:13">
       <c r="A29" s="18"/>
       <c r="B29" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C29" s="19">
         <v>0.71298700000000004</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:13">
       <c r="A30" s="15" t="s">
         <v>79</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C30" s="23">
         <v>0.103896103896103</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1">
+    <row r="31" spans="1:13" ht="15.75" thickBot="1">
       <c r="A31" s="20" t="s">
         <v>79</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C31" s="22">
         <v>0.54545454540000005</v>
@@ -2118,7 +2245,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="B36" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C36" s="11">
         <v>0.70129870129799998</v>
@@ -2126,7 +2253,7 @@
     </row>
     <row r="37" spans="1:3">
       <c r="B37" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C37">
         <v>0.70129870129799998</v>
@@ -2163,10 +2290,10 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -2181,45 +2308,45 @@
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="28" t="s">
-        <v>183</v>
+      <c r="A45" s="31" t="s">
+        <v>182</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C45">
         <v>0.64935064935064901</v>
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="28"/>
+      <c r="A46" s="31"/>
       <c r="B46" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C46">
         <v>0.662337662337662</v>
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="28"/>
+      <c r="A47" s="31"/>
       <c r="B47" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C47">
         <v>0.662337662337662</v>
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="28"/>
+      <c r="A48" s="31"/>
       <c r="B48" s="24" t="s">
         <v>77</v>
       </c>
       <c r="C48" s="11"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="28"/>
+      <c r="A49" s="31"/>
       <c r="B49" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C49">
         <v>0.72727272727299996</v>
@@ -2229,29 +2356,29 @@
       <c r="B50" s="10"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="28" t="s">
-        <v>184</v>
+      <c r="A51" s="31" t="s">
+        <v>183</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C51">
         <v>0.64935064935064901</v>
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="28"/>
+      <c r="A52" s="31"/>
       <c r="B52" s="24" t="s">
         <v>77</v>
       </c>
       <c r="C52" s="11"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="28"/>
+      <c r="A53" s="31"/>
       <c r="B53" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C53" s="29">
+        <v>91</v>
+      </c>
+      <c r="C53">
         <v>0.68831168831168799</v>
       </c>
     </row>
@@ -2264,57 +2391,58 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
+        <v>92</v>
+      </c>
+      <c r="B56" t="s">
         <v>93</v>
-      </c>
-      <c r="B56" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B57" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B58" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="10"/>
       <c r="B59" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B60" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="82" spans="1:7">
       <c r="A82" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C82" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G82" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A45:A49"/>
     <mergeCell ref="A51:A53"/>
+    <mergeCell ref="K15:M15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2338,427 +2466,427 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" s="26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="26" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" s="25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" s="25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" s="25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" s="25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" s="25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" s="25" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating working files for allgorithms 3 and 4
</commit_message>
<xml_diff>
--- a/Table of article comparision.xlsx
+++ b/Table of article comparision.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c49cb972183112a/Documents OneDrive/06 - CCT Masters in DA/Capstone - 2023/Capstone_Project_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="483" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9C1EFD6-1CDF-483F-A118-1ACAD9591E8B}"/>
+  <xr:revisionPtr revIDLastSave="489" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E49F1AC8-4F97-4D4D-A800-7B291EB37A92}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="1" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
   </bookViews>
@@ -948,18 +948,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -974,6 +962,18 @@
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1845,8 +1845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61403218-7A3E-4B26-8B7C-D3F4D407424F}">
   <dimension ref="A1:M82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2031,11 +2031,11 @@
       <c r="C15">
         <v>0.57142857000000002</v>
       </c>
-      <c r="K15" s="32" t="s">
+      <c r="K15" s="37" t="s">
         <v>199</v>
       </c>
-      <c r="L15" s="33"/>
-      <c r="M15" s="34"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="39"/>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="8" t="s">
@@ -2045,13 +2045,13 @@
         <v>0.62337662329999999</v>
       </c>
       <c r="J16" s="28"/>
-      <c r="K16" s="36" t="s">
+      <c r="K16" s="32" t="s">
         <v>197</v>
       </c>
-      <c r="L16" s="36" t="s">
+      <c r="L16" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="M16" s="36" t="s">
+      <c r="M16" s="32" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2065,13 +2065,13 @@
       <c r="J17" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="K17" s="38">
+      <c r="K17" s="34">
         <v>0.62090000000000001</v>
       </c>
-      <c r="L17" s="39">
+      <c r="L17" s="35">
         <v>0.66990000000000005</v>
       </c>
-      <c r="M17" s="37">
+      <c r="M17" s="33">
         <v>7.5200000000000003E-2</v>
       </c>
     </row>
@@ -2080,11 +2080,11 @@
       <c r="J18" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="K18" s="35">
+      <c r="K18" s="31">
         <v>0.51948051948051899</v>
       </c>
-      <c r="L18" s="37"/>
-      <c r="M18" s="37"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
@@ -2099,9 +2099,15 @@
       <c r="J19" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="K19" s="35"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
+      <c r="K19" s="31">
+        <v>0.57142857142857095</v>
+      </c>
+      <c r="L19" s="33">
+        <v>0.70129870129870098</v>
+      </c>
+      <c r="M19" s="33">
+        <v>9.0909090909090898E-2</v>
+      </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="6" t="s">
@@ -2114,9 +2120,15 @@
       <c r="J20" s="28" t="s">
         <v>194</v>
       </c>
-      <c r="K20" s="35"/>
-      <c r="L20" s="37"/>
-      <c r="M20" s="37"/>
+      <c r="K20" s="31">
+        <v>0.63636363636363602</v>
+      </c>
+      <c r="L20" s="33">
+        <v>0.70129870129870098</v>
+      </c>
+      <c r="M20" s="33">
+        <v>5.1948051948051903E-2</v>
+      </c>
     </row>
     <row r="21" spans="1:13">
       <c r="B21" t="s">
@@ -2125,9 +2137,9 @@
       <c r="J21" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="K21" s="35"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="37"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
     </row>
     <row r="22" spans="1:13">
       <c r="B22" s="24" t="s">
@@ -2308,7 +2320,7 @@
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="31" t="s">
+      <c r="A45" s="36" t="s">
         <v>182</v>
       </c>
       <c r="B45" s="10" t="s">
@@ -2319,7 +2331,7 @@
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="31"/>
+      <c r="A46" s="36"/>
       <c r="B46" s="10" t="s">
         <v>90</v>
       </c>
@@ -2328,7 +2340,7 @@
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="31"/>
+      <c r="A47" s="36"/>
       <c r="B47" s="10" t="s">
         <v>91</v>
       </c>
@@ -2337,14 +2349,14 @@
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="31"/>
+      <c r="A48" s="36"/>
       <c r="B48" s="24" t="s">
         <v>77</v>
       </c>
       <c r="C48" s="11"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="31"/>
+      <c r="A49" s="36"/>
       <c r="B49" s="10" t="s">
         <v>91</v>
       </c>
@@ -2356,7 +2368,7 @@
       <c r="B50" s="10"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="31" t="s">
+      <c r="A51" s="36" t="s">
         <v>183</v>
       </c>
       <c r="B51" s="10" t="s">
@@ -2367,14 +2379,14 @@
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="31"/>
+      <c r="A52" s="36"/>
       <c r="B52" s="24" t="s">
         <v>77</v>
       </c>
       <c r="C52" s="11"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="31"/>
+      <c r="A53" s="36"/>
       <c r="B53" s="10" t="s">
         <v>91</v>
       </c>

</xml_diff>

<commit_message>
Algorithm 5 and Report
</commit_message>
<xml_diff>
--- a/Table of article comparision.xlsx
+++ b/Table of article comparision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c49cb972183112a/Documents OneDrive/06 - CCT Masters in DA/Capstone - 2023/Capstone_Project_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="489" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E49F1AC8-4F97-4D4D-A800-7B291EB37A92}"/>
+  <xr:revisionPtr revIDLastSave="494" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0DAFB39-787D-40C7-BC60-2C6638C21407}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="1" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
+    <workbookView xWindow="630" yWindow="135" windowWidth="14460" windowHeight="15375" firstSheet="1" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison Chart" sheetId="1" r:id="rId1"/>
@@ -677,7 +677,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -720,6 +720,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -960,9 +966,6 @@
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -974,6 +977,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1845,8 +1851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61403218-7A3E-4B26-8B7C-D3F4D407424F}">
   <dimension ref="A1:M82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2031,11 +2037,11 @@
       <c r="C15">
         <v>0.57142857000000002</v>
       </c>
-      <c r="K15" s="37" t="s">
+      <c r="K15" s="36" t="s">
         <v>199</v>
       </c>
-      <c r="L15" s="38"/>
-      <c r="M15" s="39"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="38"/>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="8" t="s">
@@ -2068,7 +2074,7 @@
       <c r="K17" s="34">
         <v>0.62090000000000001</v>
       </c>
-      <c r="L17" s="35">
+      <c r="L17" s="39">
         <v>0.66990000000000005</v>
       </c>
       <c r="M17" s="33">
@@ -2320,7 +2326,7 @@
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="35" t="s">
         <v>182</v>
       </c>
       <c r="B45" s="10" t="s">
@@ -2331,7 +2337,7 @@
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="36"/>
+      <c r="A46" s="35"/>
       <c r="B46" s="10" t="s">
         <v>90</v>
       </c>
@@ -2340,7 +2346,7 @@
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="36"/>
+      <c r="A47" s="35"/>
       <c r="B47" s="10" t="s">
         <v>91</v>
       </c>
@@ -2349,14 +2355,14 @@
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="36"/>
+      <c r="A48" s="35"/>
       <c r="B48" s="24" t="s">
         <v>77</v>
       </c>
       <c r="C48" s="11"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="36"/>
+      <c r="A49" s="35"/>
       <c r="B49" s="10" t="s">
         <v>91</v>
       </c>
@@ -2368,7 +2374,7 @@
       <c r="B50" s="10"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="36" t="s">
+      <c r="A51" s="35" t="s">
         <v>183</v>
       </c>
       <c r="B51" s="10" t="s">
@@ -2379,14 +2385,14 @@
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="36"/>
+      <c r="A52" s="35"/>
       <c r="B52" s="24" t="s">
         <v>77</v>
       </c>
       <c r="C52" s="11"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="36"/>
+      <c r="A53" s="35"/>
       <c r="B53" s="10" t="s">
         <v>91</v>
       </c>

</xml_diff>

<commit_message>
Algorith 5 - run with multiple variables
</commit_message>
<xml_diff>
--- a/Table of article comparision.xlsx
+++ b/Table of article comparision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c49cb972183112a/Documents OneDrive/06 - CCT Masters in DA/Capstone - 2023/Capstone_Project_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="494" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0DAFB39-787D-40C7-BC60-2C6638C21407}"/>
+  <xr:revisionPtr revIDLastSave="502" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB1FC9F1-6FDD-451A-9249-097941E1664A}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="135" windowWidth="14460" windowHeight="15375" firstSheet="1" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
+    <workbookView xWindow="28875" yWindow="15" windowWidth="14460" windowHeight="15375" firstSheet="1" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison Chart" sheetId="1" r:id="rId1"/>
@@ -896,7 +896,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -966,6 +966,9 @@
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -978,7 +981,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1852,7 +1858,7 @@
   <dimension ref="A1:M82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2037,11 +2043,11 @@
       <c r="C15">
         <v>0.57142857000000002</v>
       </c>
-      <c r="K15" s="36" t="s">
+      <c r="K15" s="37" t="s">
         <v>199</v>
       </c>
-      <c r="L15" s="37"/>
-      <c r="M15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="39"/>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="8" t="s">
@@ -2074,7 +2080,7 @@
       <c r="K17" s="34">
         <v>0.62090000000000001</v>
       </c>
-      <c r="L17" s="39">
+      <c r="L17" s="35">
         <v>0.66990000000000005</v>
       </c>
       <c r="M17" s="33">
@@ -2089,8 +2095,8 @@
       <c r="K18" s="31">
         <v>0.51948051948051899</v>
       </c>
-      <c r="L18" s="33"/>
-      <c r="M18" s="33"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
@@ -2126,7 +2132,7 @@
       <c r="J20" s="28" t="s">
         <v>194</v>
       </c>
-      <c r="K20" s="31">
+      <c r="K20" s="41">
         <v>0.63636363636363602</v>
       </c>
       <c r="L20" s="33">
@@ -2143,9 +2149,15 @@
       <c r="J21" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="K21" s="31"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
+      <c r="K21" s="31">
+        <v>0.57142859697341897</v>
+      </c>
+      <c r="L21" s="33">
+        <v>0</v>
+      </c>
+      <c r="M21" s="41">
+        <v>0.42857143282890298</v>
+      </c>
     </row>
     <row r="22" spans="1:13">
       <c r="B22" s="24" t="s">
@@ -2326,7 +2338,7 @@
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="36" t="s">
         <v>182</v>
       </c>
       <c r="B45" s="10" t="s">
@@ -2337,7 +2349,7 @@
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="35"/>
+      <c r="A46" s="36"/>
       <c r="B46" s="10" t="s">
         <v>90</v>
       </c>
@@ -2346,7 +2358,7 @@
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="35"/>
+      <c r="A47" s="36"/>
       <c r="B47" s="10" t="s">
         <v>91</v>
       </c>
@@ -2355,14 +2367,14 @@
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="35"/>
+      <c r="A48" s="36"/>
       <c r="B48" s="24" t="s">
         <v>77</v>
       </c>
       <c r="C48" s="11"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="35"/>
+      <c r="A49" s="36"/>
       <c r="B49" s="10" t="s">
         <v>91</v>
       </c>
@@ -2374,7 +2386,7 @@
       <c r="B50" s="10"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="35" t="s">
+      <c r="A51" s="36" t="s">
         <v>183</v>
       </c>
       <c r="B51" s="10" t="s">
@@ -2385,14 +2397,14 @@
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="35"/>
+      <c r="A52" s="36"/>
       <c r="B52" s="24" t="s">
         <v>77</v>
       </c>
       <c r="C52" s="11"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="35"/>
+      <c r="A53" s="36"/>
       <c r="B53" s="10" t="s">
         <v>91</v>
       </c>

</xml_diff>

<commit_message>
Work on Chaptsers 2 and 5
</commit_message>
<xml_diff>
--- a/Table of article comparision.xlsx
+++ b/Table of article comparision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c49cb972183112a/Documents OneDrive/06 - CCT Masters in DA/Capstone - 2023/Capstone_Project_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="502" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB1FC9F1-6FDD-451A-9249-097941E1664A}"/>
+  <xr:revisionPtr revIDLastSave="509" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C02967F4-7394-40A1-9207-10DC216203C3}"/>
   <bookViews>
-    <workbookView xWindow="28875" yWindow="15" windowWidth="14460" windowHeight="15375" firstSheet="1" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
+    <workbookView xWindow="14295" yWindow="225" windowWidth="14460" windowHeight="15375" firstSheet="1" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison Chart" sheetId="1" r:id="rId1"/>
@@ -677,7 +677,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -725,6 +725,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -896,7 +907,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -954,37 +965,28 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="7" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1857,8 +1859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61403218-7A3E-4B26-8B7C-D3F4D407424F}">
   <dimension ref="A1:M82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="G7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15:M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2043,11 +2045,11 @@
       <c r="C15">
         <v>0.57142857000000002</v>
       </c>
-      <c r="K15" s="37" t="s">
+      <c r="K15" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="L15" s="38"/>
-      <c r="M15" s="39"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="37"/>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="8" t="s">
@@ -2057,13 +2059,13 @@
         <v>0.62337662329999999</v>
       </c>
       <c r="J16" s="28"/>
-      <c r="K16" s="32" t="s">
+      <c r="K16" s="38" t="s">
         <v>197</v>
       </c>
-      <c r="L16" s="32" t="s">
+      <c r="L16" s="38" t="s">
         <v>198</v>
       </c>
-      <c r="M16" s="32" t="s">
+      <c r="M16" s="38" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2077,13 +2079,13 @@
       <c r="J17" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="K17" s="34">
+      <c r="K17" s="33">
         <v>0.62090000000000001</v>
       </c>
-      <c r="L17" s="35">
+      <c r="L17" s="31">
         <v>0.66990000000000005</v>
       </c>
-      <c r="M17" s="33">
+      <c r="M17" s="31">
         <v>7.5200000000000003E-2</v>
       </c>
     </row>
@@ -2092,11 +2094,15 @@
       <c r="J18" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="K18" s="31">
+      <c r="K18" s="34">
         <v>0.51948051948051899</v>
       </c>
-      <c r="L18" s="40"/>
-      <c r="M18" s="40"/>
+      <c r="L18" s="34">
+        <v>0.70129870129870098</v>
+      </c>
+      <c r="M18" s="34">
+        <v>0.103896103896103</v>
+      </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
@@ -2111,13 +2117,13 @@
       <c r="J19" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="K19" s="31">
+      <c r="K19" s="34">
         <v>0.57142857142857095</v>
       </c>
-      <c r="L19" s="33">
+      <c r="L19" s="31">
         <v>0.70129870129870098</v>
       </c>
-      <c r="M19" s="33">
+      <c r="M19" s="31">
         <v>9.0909090909090898E-2</v>
       </c>
     </row>
@@ -2132,13 +2138,13 @@
       <c r="J20" s="28" t="s">
         <v>194</v>
       </c>
-      <c r="K20" s="41">
+      <c r="K20" s="34">
         <v>0.63636363636363602</v>
       </c>
-      <c r="L20" s="33">
+      <c r="L20" s="31">
         <v>0.70129870129870098</v>
       </c>
-      <c r="M20" s="33">
+      <c r="M20" s="31">
         <v>5.1948051948051903E-2</v>
       </c>
     </row>
@@ -2149,13 +2155,13 @@
       <c r="J21" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="K21" s="31">
+      <c r="K21" s="34">
         <v>0.57142859697341897</v>
       </c>
-      <c r="L21" s="33">
+      <c r="L21" s="31">
         <v>0</v>
       </c>
-      <c r="M21" s="41">
+      <c r="M21" s="34">
         <v>0.42857143282890298</v>
       </c>
     </row>
@@ -2338,7 +2344,7 @@
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="32" t="s">
         <v>182</v>
       </c>
       <c r="B45" s="10" t="s">
@@ -2349,7 +2355,7 @@
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="36"/>
+      <c r="A46" s="32"/>
       <c r="B46" s="10" t="s">
         <v>90</v>
       </c>
@@ -2358,7 +2364,7 @@
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="36"/>
+      <c r="A47" s="32"/>
       <c r="B47" s="10" t="s">
         <v>91</v>
       </c>
@@ -2367,14 +2373,14 @@
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="36"/>
+      <c r="A48" s="32"/>
       <c r="B48" s="24" t="s">
         <v>77</v>
       </c>
       <c r="C48" s="11"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="36"/>
+      <c r="A49" s="32"/>
       <c r="B49" s="10" t="s">
         <v>91</v>
       </c>
@@ -2386,7 +2392,7 @@
       <c r="B50" s="10"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="36" t="s">
+      <c r="A51" s="32" t="s">
         <v>183</v>
       </c>
       <c r="B51" s="10" t="s">
@@ -2397,14 +2403,14 @@
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="36"/>
+      <c r="A52" s="32"/>
       <c r="B52" s="24" t="s">
         <v>77</v>
       </c>
       <c r="C52" s="11"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="36"/>
+      <c r="A53" s="32"/>
       <c r="B53" s="10" t="s">
         <v>91</v>
       </c>

</xml_diff>

<commit_message>
Implement test data on Algorithm 2
</commit_message>
<xml_diff>
--- a/Table of article comparision.xlsx
+++ b/Table of article comparision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c49cb972183112a/Documents OneDrive/06 - CCT Masters in DA/Capstone - 2023/Capstone_Project_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="509" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C02967F4-7394-40A1-9207-10DC216203C3}"/>
+  <xr:revisionPtr revIDLastSave="524" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94A0DDFA-D3A6-48D9-A6D2-6AC45ECF017F}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="225" windowWidth="14460" windowHeight="15375" firstSheet="1" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="1" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison Chart" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="202">
   <si>
     <t>Authors</t>
   </si>
@@ -668,6 +668,9 @@
   </si>
   <si>
     <t>Decision Tree - categorical data</t>
+  </si>
+  <si>
+    <t>Accuracy results using Test Data</t>
   </si>
 </sst>
 </file>
@@ -742,7 +745,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -758,6 +761,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -907,7 +916,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -968,13 +977,16 @@
     <xf numFmtId="10" fontId="7" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="7" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -986,7 +998,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1857,10 +1884,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61403218-7A3E-4B26-8B7C-D3F4D407424F}">
-  <dimension ref="A1:M82"/>
+  <dimension ref="A1:P82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15:M21"/>
+    <sheetView tabSelected="1" topLeftCell="G4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1876,9 +1903,12 @@
     <col min="11" max="11" width="16.85546875" customWidth="1"/>
     <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.140625" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -1886,7 +1916,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:16">
       <c r="A2" s="6" t="s">
         <v>79</v>
       </c>
@@ -1900,7 +1930,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:16">
       <c r="B3" t="s">
         <v>55</v>
       </c>
@@ -1911,12 +1941,12 @@
         <v>0.57142899999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:16">
       <c r="B4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:16">
       <c r="B5" t="s">
         <v>62</v>
       </c>
@@ -1927,7 +1957,7 @@
         <v>0.57142899999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:16">
       <c r="B6" t="s">
         <v>63</v>
       </c>
@@ -1938,7 +1968,7 @@
         <v>0.57142899999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:16">
       <c r="B7" t="s">
         <v>64</v>
       </c>
@@ -1953,7 +1983,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:16">
       <c r="B8" t="s">
         <v>65</v>
       </c>
@@ -1970,7 +2000,7 @@
         <v>0.62091499999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:16">
       <c r="J9" s="28" t="s">
         <v>192</v>
       </c>
@@ -1978,7 +2008,7 @@
         <v>0.71298700000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -1993,7 +2023,7 @@
         <v>0.70129870129799998</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:16">
       <c r="A11" s="6" t="s">
         <v>79</v>
       </c>
@@ -2010,7 +2040,7 @@
         <v>0.72727272727299996</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:16">
       <c r="B12" t="s">
         <v>55</v>
       </c>
@@ -2024,13 +2054,13 @@
         <v>0.66993499999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:16">
       <c r="B13" t="s">
         <v>61</v>
       </c>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:16">
       <c r="B14" s="7" t="s">
         <v>67</v>
       </c>
@@ -2038,20 +2068,25 @@
         <v>0.61038899999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:16">
       <c r="B15" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C15">
         <v>0.57142857000000002</v>
       </c>
-      <c r="K15" s="35" t="s">
+      <c r="K15" s="36" t="s">
         <v>199</v>
       </c>
-      <c r="L15" s="36"/>
-      <c r="M15" s="37"/>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="L15" s="37"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="42" t="s">
+        <v>201</v>
+      </c>
+      <c r="O15" s="42"/>
+      <c r="P15" s="42"/>
+    </row>
+    <row r="16" spans="1:16">
       <c r="B16" s="8" t="s">
         <v>69</v>
       </c>
@@ -2059,17 +2094,26 @@
         <v>0.62337662329999999</v>
       </c>
       <c r="J16" s="28"/>
-      <c r="K16" s="38" t="s">
+      <c r="K16" s="34" t="s">
         <v>197</v>
       </c>
-      <c r="L16" s="38" t="s">
+      <c r="L16" s="34" t="s">
         <v>198</v>
       </c>
-      <c r="M16" s="38" t="s">
+      <c r="M16" s="34" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="N16" s="41" t="s">
+        <v>197</v>
+      </c>
+      <c r="O16" s="41" t="s">
+        <v>198</v>
+      </c>
+      <c r="P16" s="41" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="B17" s="7" t="s">
         <v>66</v>
       </c>
@@ -2079,7 +2123,7 @@
       <c r="J17" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="K17" s="33">
+      <c r="K17" s="32">
         <v>0.62090000000000001</v>
       </c>
       <c r="L17" s="31">
@@ -2088,23 +2132,35 @@
       <c r="M17" s="31">
         <v>7.5200000000000003E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="N17" s="43"/>
+      <c r="O17" s="43"/>
+      <c r="P17" s="43"/>
+    </row>
+    <row r="18" spans="1:16">
       <c r="B18" s="7"/>
-      <c r="J18" s="28" t="s">
+      <c r="J18" s="39" t="s">
         <v>192</v>
       </c>
-      <c r="K18" s="34">
+      <c r="K18" s="40">
         <v>0.51948051948051899</v>
       </c>
-      <c r="L18" s="34">
+      <c r="L18" s="40">
         <v>0.70129870129870098</v>
       </c>
-      <c r="M18" s="34">
+      <c r="M18" s="40">
         <v>0.103896103896103</v>
       </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="N18" s="44">
+        <v>0.793333333333333</v>
+      </c>
+      <c r="O18" s="44">
+        <v>0.92</v>
+      </c>
+      <c r="P18" s="44">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -2114,20 +2170,23 @@
       <c r="C19" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="J19" s="28" t="s">
+      <c r="J19" s="39" t="s">
         <v>193</v>
       </c>
-      <c r="K19" s="34">
+      <c r="K19" s="40">
         <v>0.57142857142857095</v>
       </c>
-      <c r="L19" s="31">
+      <c r="L19" s="40">
         <v>0.70129870129870098</v>
       </c>
-      <c r="M19" s="31">
+      <c r="M19" s="40">
         <v>9.0909090909090898E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="N19" s="43"/>
+      <c r="O19" s="43"/>
+      <c r="P19" s="43"/>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" s="6" t="s">
         <v>79</v>
       </c>
@@ -2135,37 +2194,43 @@
         <v>60</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="J20" s="28" t="s">
+      <c r="J20" s="39" t="s">
         <v>194</v>
       </c>
-      <c r="K20" s="34">
+      <c r="K20" s="40">
         <v>0.63636363636363602</v>
       </c>
-      <c r="L20" s="31">
+      <c r="L20" s="40">
         <v>0.70129870129870098</v>
       </c>
-      <c r="M20" s="31">
+      <c r="M20" s="40">
         <v>5.1948051948051903E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="N20" s="43"/>
+      <c r="O20" s="43"/>
+      <c r="P20" s="43"/>
+    </row>
+    <row r="21" spans="1:16">
       <c r="B21" t="s">
         <v>61</v>
       </c>
       <c r="J21" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="K21" s="34">
+      <c r="K21" s="33">
         <v>0.57142859697341897</v>
       </c>
       <c r="L21" s="31">
         <v>0</v>
       </c>
-      <c r="M21" s="34">
+      <c r="M21" s="33">
         <v>0.42857143282890298</v>
       </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="N21" s="43"/>
+      <c r="O21" s="43"/>
+      <c r="P21" s="43"/>
+    </row>
+    <row r="22" spans="1:16">
       <c r="B22" s="24" t="s">
         <v>66</v>
       </c>
@@ -2173,7 +2238,7 @@
         <v>0.62337662329999999</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:16">
       <c r="B23" s="7" t="s">
         <v>67</v>
       </c>
@@ -2181,7 +2246,7 @@
         <v>0.61038899999999996</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:16">
       <c r="B24" s="7" t="s">
         <v>68</v>
       </c>
@@ -2189,10 +2254,10 @@
         <v>0.57142857000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="15.75" thickBot="1">
+    <row r="25" spans="1:16" ht="15.75" thickBot="1">
       <c r="B25" s="7"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:16">
       <c r="A26" s="12" t="s">
         <v>59</v>
       </c>
@@ -2201,7 +2266,7 @@
       </c>
       <c r="C26" s="14"/>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:16">
       <c r="A27" s="15" t="s">
         <v>79</v>
       </c>
@@ -2212,7 +2277,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:16">
       <c r="A28" s="15"/>
       <c r="B28" s="10" t="s">
         <v>55</v>
@@ -2221,7 +2286,7 @@
         <v>0.57142857142000003</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:16">
       <c r="A29" s="18"/>
       <c r="B29" s="11" t="s">
         <v>82</v>
@@ -2230,7 +2295,7 @@
         <v>0.71298700000000004</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:16">
       <c r="A30" s="15" t="s">
         <v>79</v>
       </c>
@@ -2241,7 +2306,7 @@
         <v>0.103896103896103</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="15.75" thickBot="1">
+    <row r="31" spans="1:16" ht="15.75" thickBot="1">
       <c r="A31" s="20" t="s">
         <v>79</v>
       </c>
@@ -2344,7 +2409,7 @@
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="32" t="s">
+      <c r="A45" s="35" t="s">
         <v>182</v>
       </c>
       <c r="B45" s="10" t="s">
@@ -2355,7 +2420,7 @@
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="32"/>
+      <c r="A46" s="35"/>
       <c r="B46" s="10" t="s">
         <v>90</v>
       </c>
@@ -2364,7 +2429,7 @@
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="32"/>
+      <c r="A47" s="35"/>
       <c r="B47" s="10" t="s">
         <v>91</v>
       </c>
@@ -2373,14 +2438,14 @@
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="32"/>
+      <c r="A48" s="35"/>
       <c r="B48" s="24" t="s">
         <v>77</v>
       </c>
       <c r="C48" s="11"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="32"/>
+      <c r="A49" s="35"/>
       <c r="B49" s="10" t="s">
         <v>91</v>
       </c>
@@ -2392,7 +2457,7 @@
       <c r="B50" s="10"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="32" t="s">
+      <c r="A51" s="35" t="s">
         <v>183</v>
       </c>
       <c r="B51" s="10" t="s">
@@ -2403,14 +2468,14 @@
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="32"/>
+      <c r="A52" s="35"/>
       <c r="B52" s="24" t="s">
         <v>77</v>
       </c>
       <c r="C52" s="11"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="32"/>
+      <c r="A53" s="35"/>
       <c r="B53" s="10" t="s">
         <v>91</v>
       </c>
@@ -2475,10 +2540,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A45:A49"/>
     <mergeCell ref="A51:A53"/>
     <mergeCell ref="K15:M15"/>
+    <mergeCell ref="N15:P15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Running test data on algorithms 3 and 4
</commit_message>
<xml_diff>
--- a/Table of article comparision.xlsx
+++ b/Table of article comparision.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c49cb972183112a/Documents OneDrive/06 - CCT Masters in DA/Capstone - 2023/Capstone_Project_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="524" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94A0DDFA-D3A6-48D9-A6D2-6AC45ECF017F}"/>
+  <xr:revisionPtr revIDLastSave="545" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F047B409-9633-4AD0-8CBC-F9D582AA69EE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="1" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
   </bookViews>
@@ -986,6 +986,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -998,22 +1007,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="7" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1886,8 +1886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61403218-7A3E-4B26-8B7C-D3F4D407424F}">
   <dimension ref="A1:P82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2075,11 +2075,11 @@
       <c r="C15">
         <v>0.57142857000000002</v>
       </c>
-      <c r="K15" s="36" t="s">
+      <c r="K15" s="39" t="s">
         <v>199</v>
       </c>
-      <c r="L15" s="37"/>
-      <c r="M15" s="38"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="41"/>
       <c r="N15" s="42" t="s">
         <v>201</v>
       </c>
@@ -2103,13 +2103,13 @@
       <c r="M16" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="N16" s="41" t="s">
+      <c r="N16" s="37" t="s">
         <v>197</v>
       </c>
-      <c r="O16" s="41" t="s">
+      <c r="O16" s="37" t="s">
         <v>198</v>
       </c>
-      <c r="P16" s="41" t="s">
+      <c r="P16" s="37" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2138,16 +2138,16 @@
     </row>
     <row r="18" spans="1:16">
       <c r="B18" s="7"/>
-      <c r="J18" s="39" t="s">
+      <c r="J18" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="K18" s="40">
+      <c r="K18" s="36">
         <v>0.51948051948051899</v>
       </c>
-      <c r="L18" s="40">
+      <c r="L18" s="36">
         <v>0.70129870129870098</v>
       </c>
-      <c r="M18" s="40">
+      <c r="M18" s="36">
         <v>0.103896103896103</v>
       </c>
       <c r="N18" s="44">
@@ -2170,21 +2170,27 @@
       <c r="C19" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="J19" s="39" t="s">
+      <c r="J19" s="35" t="s">
         <v>193</v>
       </c>
-      <c r="K19" s="40">
-        <v>0.57142857142857095</v>
-      </c>
-      <c r="L19" s="40">
-        <v>0.70129870129870098</v>
-      </c>
-      <c r="M19" s="40">
-        <v>9.0909090909090898E-2</v>
-      </c>
-      <c r="N19" s="43"/>
-      <c r="O19" s="43"/>
-      <c r="P19" s="43"/>
+      <c r="K19" s="36">
+        <v>0.57142899999999996</v>
+      </c>
+      <c r="L19" s="36">
+        <v>0.67532499999999995</v>
+      </c>
+      <c r="M19" s="36">
+        <v>5.1948099999999997E-2</v>
+      </c>
+      <c r="N19" s="43">
+        <v>0.206666666666666</v>
+      </c>
+      <c r="O19" s="43">
+        <v>0.92</v>
+      </c>
+      <c r="P19" s="43">
+        <v>2.6666666666666599E-2</v>
+      </c>
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="6" t="s">
@@ -2194,21 +2200,27 @@
         <v>60</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="J20" s="39" t="s">
+      <c r="J20" s="35" t="s">
         <v>194</v>
       </c>
-      <c r="K20" s="40">
+      <c r="K20" s="36">
         <v>0.63636363636363602</v>
       </c>
-      <c r="L20" s="40">
+      <c r="L20" s="36">
         <v>0.70129870129870098</v>
       </c>
-      <c r="M20" s="40">
+      <c r="M20" s="36">
         <v>5.1948051948051903E-2</v>
       </c>
-      <c r="N20" s="43"/>
-      <c r="O20" s="43"/>
-      <c r="P20" s="43"/>
+      <c r="N20" s="43">
+        <v>0.793333333333333</v>
+      </c>
+      <c r="O20" s="43">
+        <v>0.92</v>
+      </c>
+      <c r="P20" s="43">
+        <v>4.6666699999999998E-2</v>
+      </c>
     </row>
     <row r="21" spans="1:16">
       <c r="B21" t="s">
@@ -2409,7 +2421,7 @@
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="38" t="s">
         <v>182</v>
       </c>
       <c r="B45" s="10" t="s">
@@ -2420,7 +2432,7 @@
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="35"/>
+      <c r="A46" s="38"/>
       <c r="B46" s="10" t="s">
         <v>90</v>
       </c>
@@ -2429,7 +2441,7 @@
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="35"/>
+      <c r="A47" s="38"/>
       <c r="B47" s="10" t="s">
         <v>91</v>
       </c>
@@ -2438,14 +2450,14 @@
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="35"/>
+      <c r="A48" s="38"/>
       <c r="B48" s="24" t="s">
         <v>77</v>
       </c>
       <c r="C48" s="11"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="35"/>
+      <c r="A49" s="38"/>
       <c r="B49" s="10" t="s">
         <v>91</v>
       </c>
@@ -2457,7 +2469,7 @@
       <c r="B50" s="10"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="35" t="s">
+      <c r="A51" s="38" t="s">
         <v>183</v>
       </c>
       <c r="B51" s="10" t="s">
@@ -2468,14 +2480,14 @@
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="35"/>
+      <c r="A52" s="38"/>
       <c r="B52" s="24" t="s">
         <v>77</v>
       </c>
       <c r="C52" s="11"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="35"/>
+      <c r="A53" s="38"/>
       <c r="B53" s="10" t="s">
         <v>91</v>
       </c>

</xml_diff>

<commit_message>
Rework of Chapter 3
</commit_message>
<xml_diff>
--- a/Table of article comparision.xlsx
+++ b/Table of article comparision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c49cb972183112a/Documents OneDrive/06 - CCT Masters in DA/Capstone - 2023/Capstone_Project_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="545" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F047B409-9633-4AD0-8CBC-F9D582AA69EE}"/>
+  <xr:revisionPtr revIDLastSave="549" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9D54BF1-C201-48C9-8D26-55BBFEE68AB0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="1" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison Chart" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="203">
   <si>
     <t>Authors</t>
   </si>
@@ -671,6 +671,9 @@
   </si>
   <si>
     <t>Accuracy results using Test Data</t>
+  </si>
+  <si>
+    <t>Josh Bersin</t>
   </si>
 </sst>
 </file>
@@ -995,6 +998,12 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1009,12 +1018,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1519,11 +1522,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:G16"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1833,47 +1836,25 @@
       <c r="A15" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="2">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="2">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="2">
-        <v>20</v>
-      </c>
-      <c r="B21" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5" t="s">
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1886,7 +1867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61403218-7A3E-4B26-8B7C-D3F4D407424F}">
   <dimension ref="A1:P82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
@@ -2075,16 +2056,16 @@
       <c r="C15">
         <v>0.57142857000000002</v>
       </c>
-      <c r="K15" s="39" t="s">
+      <c r="K15" s="41" t="s">
         <v>199</v>
       </c>
-      <c r="L15" s="40"/>
-      <c r="M15" s="41"/>
-      <c r="N15" s="42" t="s">
+      <c r="L15" s="42"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="44" t="s">
         <v>201</v>
       </c>
-      <c r="O15" s="42"/>
-      <c r="P15" s="42"/>
+      <c r="O15" s="44"/>
+      <c r="P15" s="44"/>
     </row>
     <row r="16" spans="1:16">
       <c r="B16" s="8" t="s">
@@ -2132,9 +2113,9 @@
       <c r="M17" s="31">
         <v>7.5200000000000003E-2</v>
       </c>
-      <c r="N17" s="43"/>
-      <c r="O17" s="43"/>
-      <c r="P17" s="43"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="38"/>
     </row>
     <row r="18" spans="1:16">
       <c r="B18" s="7"/>
@@ -2150,13 +2131,13 @@
       <c r="M18" s="36">
         <v>0.103896103896103</v>
       </c>
-      <c r="N18" s="44">
+      <c r="N18" s="39">
         <v>0.793333333333333</v>
       </c>
-      <c r="O18" s="44">
+      <c r="O18" s="39">
         <v>0.92</v>
       </c>
-      <c r="P18" s="44">
+      <c r="P18" s="39">
         <v>0.04</v>
       </c>
     </row>
@@ -2182,13 +2163,13 @@
       <c r="M19" s="36">
         <v>5.1948099999999997E-2</v>
       </c>
-      <c r="N19" s="43">
+      <c r="N19" s="38">
         <v>0.206666666666666</v>
       </c>
-      <c r="O19" s="43">
+      <c r="O19" s="38">
         <v>0.92</v>
       </c>
-      <c r="P19" s="43">
+      <c r="P19" s="38">
         <v>2.6666666666666599E-2</v>
       </c>
     </row>
@@ -2212,13 +2193,13 @@
       <c r="M20" s="36">
         <v>5.1948051948051903E-2</v>
       </c>
-      <c r="N20" s="43">
+      <c r="N20" s="38">
         <v>0.793333333333333</v>
       </c>
-      <c r="O20" s="43">
+      <c r="O20" s="38">
         <v>0.92</v>
       </c>
-      <c r="P20" s="43">
+      <c r="P20" s="38">
         <v>4.6666699999999998E-2</v>
       </c>
     </row>
@@ -2238,9 +2219,9 @@
       <c r="M21" s="33">
         <v>0.42857143282890298</v>
       </c>
-      <c r="N21" s="43"/>
-      <c r="O21" s="43"/>
-      <c r="P21" s="43"/>
+      <c r="N21" s="38"/>
+      <c r="O21" s="38"/>
+      <c r="P21" s="38"/>
     </row>
     <row r="22" spans="1:16">
       <c r="B22" s="24" t="s">
@@ -2421,7 +2402,7 @@
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="38" t="s">
+      <c r="A45" s="40" t="s">
         <v>182</v>
       </c>
       <c r="B45" s="10" t="s">
@@ -2432,7 +2413,7 @@
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="38"/>
+      <c r="A46" s="40"/>
       <c r="B46" s="10" t="s">
         <v>90</v>
       </c>
@@ -2441,7 +2422,7 @@
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="38"/>
+      <c r="A47" s="40"/>
       <c r="B47" s="10" t="s">
         <v>91</v>
       </c>
@@ -2450,14 +2431,14 @@
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="38"/>
+      <c r="A48" s="40"/>
       <c r="B48" s="24" t="s">
         <v>77</v>
       </c>
       <c r="C48" s="11"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="38"/>
+      <c r="A49" s="40"/>
       <c r="B49" s="10" t="s">
         <v>91</v>
       </c>
@@ -2469,7 +2450,7 @@
       <c r="B50" s="10"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="38" t="s">
+      <c r="A51" s="40" t="s">
         <v>183</v>
       </c>
       <c r="B51" s="10" t="s">
@@ -2480,14 +2461,14 @@
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="38"/>
+      <c r="A52" s="40"/>
       <c r="B52" s="24" t="s">
         <v>77</v>
       </c>
       <c r="C52" s="11"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="38"/>
+      <c r="A53" s="40"/>
       <c r="B53" s="10" t="s">
         <v>91</v>
       </c>

</xml_diff>

<commit_message>
Chapter 3 Chapter 4
Completion of Chapter 3 and initial work on Chapt 4
</commit_message>
<xml_diff>
--- a/Table of article comparision.xlsx
+++ b/Table of article comparision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c49cb972183112a/Documents OneDrive/06 - CCT Masters in DA/Capstone - 2023/Capstone_Project_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="549" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9D54BF1-C201-48C9-8D26-55BBFEE68AB0}"/>
+  <xr:revisionPtr revIDLastSave="557" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F5527C5-5499-4463-9FD6-046A9C1255A7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison Chart" sheetId="1" r:id="rId1"/>
@@ -1180,7 +1180,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>623277</xdr:colOff>
+      <xdr:colOff>594702</xdr:colOff>
       <xdr:row>100</xdr:row>
       <xdr:rowOff>75762</xdr:rowOff>
     </xdr:to>
@@ -1524,8 +1524,8 @@
   </sheetPr>
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -1867,8 +1867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61403218-7A3E-4B26-8B7C-D3F4D407424F}">
   <dimension ref="A1:P82"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView tabSelected="1" topLeftCell="G7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15:P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1880,11 +1880,12 @@
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.42578125" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="40.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
     <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" customWidth="1"/>
-    <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" customWidth="1"/>
     <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Chapter 5 review and update of chapter 6
</commit_message>
<xml_diff>
--- a/Table of article comparision.xlsx
+++ b/Table of article comparision.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c49cb972183112a/Documents OneDrive/06 - CCT Masters in DA/Capstone - 2023/Capstone_Project_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="557" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F5527C5-5499-4463-9FD6-046A9C1255A7}"/>
+  <xr:revisionPtr revIDLastSave="601" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37F2FE93-1EBF-4145-BB06-1FF81ABD9797}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison Chart" sheetId="1" r:id="rId1"/>
     <sheet name="Algorithm Results" sheetId="2" r:id="rId2"/>
     <sheet name="Algorithm 5 - MLP" sheetId="3" r:id="rId3"/>
+    <sheet name="Graphing the Results " sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="206">
   <si>
     <t>Authors</t>
   </si>
@@ -674,6 +675,15 @@
   </si>
   <si>
     <t>Josh Bersin</t>
+  </si>
+  <si>
+    <t>Tenure -test</t>
+  </si>
+  <si>
+    <t>Studied_Credits - test</t>
+  </si>
+  <si>
+    <t>Gender - test</t>
   </si>
 </sst>
 </file>
@@ -1037,6 +1047,2917 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IE"/>
+              <a:t>Accuracy Results</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IE" baseline="0"/>
+              <a:t> by Gender</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IE"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graphing the Results '!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gender</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Graphing the Results '!$B$5:$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Algorithm 1 - Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Algorithm 2 - Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Algorithm 3 - Support Vector Machines (SVM)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Algorithm 4 - Random Forest </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Algorithm5 - Multi-Layer Perceptron (MLP)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Graphing the Results '!$C$5:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.62090000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.51948051948051899</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.57142899999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.63636363636363602</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.57142859697341897</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E0A5-4104-A740-D44CEFE5E72F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graphing the Results '!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gender - test</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Graphing the Results '!$B$5:$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Algorithm 1 - Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Algorithm 2 - Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Algorithm 3 - Support Vector Machines (SVM)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Algorithm 4 - Random Forest </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Algorithm5 - Multi-Layer Perceptron (MLP)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Graphing the Results '!$D$5:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>0.793333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.206666666666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.793333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E0A5-4104-A740-D44CEFE5E72F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1184244640"/>
+        <c:axId val="816155808"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1184244640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="816155808"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="816155808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1184244640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IE" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Accuracy Results by Studied_Credits</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graphing the Results '!$C$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Studied_Credits</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Graphing the Results '!$B$17:$B$21</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Algorithm 1 - Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Algorithm 2 - Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Algorithm 3 - Support Vector Machines (SVM)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Algorithm 4 - Random Forest </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Algorithm5 - Multi-Layer Perceptron (MLP)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Graphing the Results '!$C$17:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.66990000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.70129870129870098</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.67532499999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.70129870129870098</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E593-4599-BF9E-5925E7AE2103}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graphing the Results '!$D$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Studied_Credits - test</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Graphing the Results '!$B$17:$B$21</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Algorithm 1 - Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Algorithm 2 - Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Algorithm 3 - Support Vector Machines (SVM)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Algorithm 4 - Random Forest </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Algorithm5 - Multi-Layer Perceptron (MLP)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Graphing the Results '!$D$17:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.92</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E593-4599-BF9E-5925E7AE2103}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1182609840"/>
+        <c:axId val="696097760"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1182609840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="696097760"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="696097760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1182609840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IE" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Accuracy Results by Tenure</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graphing the Results '!$C$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tenure</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Graphing the Results '!$B$29:$B$33</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Algorithm 1 - Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Algorithm 2 - Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Algorithm 3 - Support Vector Machines (SVM)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Algorithm 4 - Random Forest </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Algorithm5 - Multi-Layer Perceptron (MLP)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Graphing the Results '!$C$29:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7.5200000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.103896103896103</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.1948099999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1948051948051903E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42857143282890298</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B46D-4A21-A5B5-07F520C20AE5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graphing the Results '!$D$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tenure -test</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Graphing the Results '!$B$29:$B$33</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Algorithm 1 - Logistic Regression</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Algorithm 2 - Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Algorithm 3 - Support Vector Machines (SVM)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Algorithm 4 - Random Forest </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Algorithm5 - Multi-Layer Perceptron (MLP)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Graphing the Results '!$D$29:$D$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6666666666666599E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.6666699999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B46D-4A21-A5B5-07F520C20AE5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="1309770048"/>
+        <c:axId val="1351453008"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1309770048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1351453008"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1351453008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1309770048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -1213,6 +4134,119 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{969CAE62-5457-E72F-9CE7-4868A7CD1974}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>43702</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>80682</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>348502</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>156882</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89A71F66-F383-8685-EE85-57D2C1CBAA85}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01C023B6-2DA4-81EC-6A2B-E65A7F488786}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1525,7 +4559,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -1867,8 +4901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61403218-7A3E-4B26-8B7C-D3F4D407424F}">
   <dimension ref="A1:P82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15:P21"/>
+    <sheetView topLeftCell="G7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2988,4 +6022,206 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AF06F93-5909-4560-A480-0827EF86C188}">
+  <dimension ref="B4:D33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:4">
+      <c r="B4" s="28"/>
+      <c r="C4" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="C5" s="32">
+        <v>0.62090000000000001</v>
+      </c>
+      <c r="D5" s="38"/>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="35" t="s">
+        <v>192</v>
+      </c>
+      <c r="C6" s="36">
+        <v>0.51948051948051899</v>
+      </c>
+      <c r="D6" s="39">
+        <v>0.793333333333333</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="C7" s="36">
+        <v>0.57142899999999996</v>
+      </c>
+      <c r="D7" s="38">
+        <v>0.206666666666666</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="C8" s="36">
+        <v>0.63636363636363602</v>
+      </c>
+      <c r="D8" s="38">
+        <v>0.793333333333333</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="C9" s="33">
+        <v>0.57142859697341897</v>
+      </c>
+      <c r="D9" s="38"/>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="28"/>
+      <c r="C16" s="34" t="s">
+        <v>198</v>
+      </c>
+      <c r="D16" s="37" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="C17" s="31">
+        <v>0.66990000000000005</v>
+      </c>
+      <c r="D17" s="38"/>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="35" t="s">
+        <v>192</v>
+      </c>
+      <c r="C18" s="36">
+        <v>0.70129870129870098</v>
+      </c>
+      <c r="D18" s="39">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="C19" s="36">
+        <v>0.67532499999999995</v>
+      </c>
+      <c r="D19" s="38">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="C20" s="36">
+        <v>0.70129870129870098</v>
+      </c>
+      <c r="D20" s="38">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="C21" s="31">
+        <v>0</v>
+      </c>
+      <c r="D21" s="38"/>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="28"/>
+      <c r="C28" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="37" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="C29" s="31">
+        <v>7.5200000000000003E-2</v>
+      </c>
+      <c r="D29" s="38"/>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" s="35" t="s">
+        <v>192</v>
+      </c>
+      <c r="C30" s="36">
+        <v>0.103896103896103</v>
+      </c>
+      <c r="D30" s="39">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="C31" s="36">
+        <v>5.1948099999999997E-2</v>
+      </c>
+      <c r="D31" s="38">
+        <v>2.6666666666666599E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="C32" s="36">
+        <v>5.1948051948051903E-2</v>
+      </c>
+      <c r="D32" s="38">
+        <v>4.6666699999999998E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="C33" s="33">
+        <v>0.42857143282890298</v>
+      </c>
+      <c r="D33" s="38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Drafts of Chapters 6 and 7
Rerun algorithm 1 for test data
</commit_message>
<xml_diff>
--- a/Table of article comparision.xlsx
+++ b/Table of article comparision.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c49cb972183112a/Documents OneDrive/06 - CCT Masters in DA/Capstone - 2023/Capstone_Project_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="601" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37F2FE93-1EBF-4145-BB06-1FF81ABD9797}"/>
+  <xr:revisionPtr revIDLastSave="636" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{423AE944-4C86-480A-97AE-5B8FE3BF8CFD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison Chart" sheetId="1" r:id="rId1"/>
     <sheet name="Algorithm Results" sheetId="2" r:id="rId2"/>
-    <sheet name="Algorithm 5 - MLP" sheetId="3" r:id="rId3"/>
-    <sheet name="Graphing the Results " sheetId="4" r:id="rId4"/>
+    <sheet name="Graphing the Results " sheetId="4" r:id="rId3"/>
+    <sheet name="Algorithm 5 - MLP" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="207">
   <si>
     <t>Authors</t>
   </si>
@@ -684,6 +684,9 @@
   </si>
   <si>
     <t>Gender - test</t>
+  </si>
+  <si>
+    <t>Algorithm 5 - Multi-Layer Perceptron (MLP)</t>
   </si>
 </sst>
 </file>
@@ -929,7 +932,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1028,6 +1031,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1258,6 +1270,9 @@
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.793333333333333</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>0.793333333333333</c:v>
                 </c:pt>
@@ -1684,6 +1699,9 @@
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.793333333333333</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>0.92</c:v>
                 </c:pt>
@@ -2023,7 +2041,7 @@
                   <c:v>Algorithm 4 - Random Forest </c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Algorithm5 - Multi-Layer Perceptron (MLP)</c:v>
+                  <c:v>Algorithm 5 - Multi-Layer Perceptron (MLP)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2035,7 +2053,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>7.5200000000000003E-2</c:v>
+                  <c:v>9.0909100000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.103896103896103</c:v>
@@ -2100,7 +2118,7 @@
                   <c:v>Algorithm 4 - Random Forest </c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Algorithm5 - Multi-Layer Perceptron (MLP)</c:v>
+                  <c:v>Algorithm 5 - Multi-Layer Perceptron (MLP)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2111,6 +2129,9 @@
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>0.04</c:v>
                 </c:pt>
@@ -4901,8 +4922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61403218-7A3E-4B26-8B7C-D3F4D407424F}">
   <dimension ref="A1:P82"/>
   <sheetViews>
-    <sheetView topLeftCell="G7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" topLeftCell="E6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20:M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5139,31 +5160,37 @@
       <c r="J17" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="K17" s="32">
+      <c r="K17" s="33">
         <v>0.62090000000000001</v>
       </c>
-      <c r="L17" s="31">
+      <c r="L17" s="33">
         <v>0.66990000000000005</v>
       </c>
-      <c r="M17" s="31">
-        <v>7.5200000000000003E-2</v>
-      </c>
-      <c r="N17" s="38"/>
-      <c r="O17" s="38"/>
-      <c r="P17" s="38"/>
+      <c r="M17" s="33">
+        <v>9.0909100000000007E-2</v>
+      </c>
+      <c r="N17" s="39">
+        <v>0.793333333333333</v>
+      </c>
+      <c r="O17" s="39">
+        <v>0.793333333333333</v>
+      </c>
+      <c r="P17" s="38">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:16">
       <c r="B18" s="7"/>
-      <c r="J18" s="35" t="s">
+      <c r="J18" s="45" t="s">
         <v>192</v>
       </c>
-      <c r="K18" s="36">
+      <c r="K18" s="33">
         <v>0.51948051948051899</v>
       </c>
-      <c r="L18" s="36">
+      <c r="L18" s="33">
         <v>0.70129870129870098</v>
       </c>
-      <c r="M18" s="36">
+      <c r="M18" s="33">
         <v>0.103896103896103</v>
       </c>
       <c r="N18" s="39">
@@ -5186,16 +5213,16 @@
       <c r="C19" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="J19" s="35" t="s">
+      <c r="J19" s="45" t="s">
         <v>193</v>
       </c>
-      <c r="K19" s="36">
+      <c r="K19" s="33">
         <v>0.57142899999999996</v>
       </c>
-      <c r="L19" s="36">
+      <c r="L19" s="33">
         <v>0.67532499999999995</v>
       </c>
-      <c r="M19" s="36">
+      <c r="M19" s="33">
         <v>5.1948099999999997E-2</v>
       </c>
       <c r="N19" s="38">
@@ -5216,16 +5243,16 @@
         <v>60</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="J20" s="35" t="s">
+      <c r="J20" s="46" t="s">
         <v>194</v>
       </c>
-      <c r="K20" s="36">
+      <c r="K20" s="47">
         <v>0.63636363636363602</v>
       </c>
-      <c r="L20" s="36">
+      <c r="L20" s="47">
         <v>0.70129870129870098</v>
       </c>
-      <c r="M20" s="36">
+      <c r="M20" s="47">
         <v>5.1948051948051903E-2</v>
       </c>
       <c r="N20" s="38">
@@ -5248,7 +5275,7 @@
       <c r="K21" s="33">
         <v>0.57142859697341897</v>
       </c>
-      <c r="L21" s="31">
+      <c r="L21" s="33">
         <v>0</v>
       </c>
       <c r="M21" s="33">
@@ -5582,6 +5609,214 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AF06F93-5909-4560-A480-0827EF86C188}">
+  <dimension ref="B4:D33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:4">
+      <c r="B4" s="28"/>
+      <c r="C4" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="C5" s="32">
+        <v>0.62090000000000001</v>
+      </c>
+      <c r="D5" s="39">
+        <v>0.793333333333333</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="35" t="s">
+        <v>192</v>
+      </c>
+      <c r="C6" s="36">
+        <v>0.51948051948051899</v>
+      </c>
+      <c r="D6" s="39">
+        <v>0.793333333333333</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="C7" s="36">
+        <v>0.57142899999999996</v>
+      </c>
+      <c r="D7" s="38">
+        <v>0.206666666666666</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="C8" s="36">
+        <v>0.63636363636363602</v>
+      </c>
+      <c r="D8" s="38">
+        <v>0.793333333333333</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="C9" s="33">
+        <v>0.57142859697341897</v>
+      </c>
+      <c r="D9" s="38"/>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="28"/>
+      <c r="C16" s="34" t="s">
+        <v>198</v>
+      </c>
+      <c r="D16" s="37" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="C17" s="31">
+        <v>0.66990000000000005</v>
+      </c>
+      <c r="D17" s="39">
+        <v>0.793333333333333</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="35" t="s">
+        <v>192</v>
+      </c>
+      <c r="C18" s="36">
+        <v>0.70129870129870098</v>
+      </c>
+      <c r="D18" s="39">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="C19" s="36">
+        <v>0.67532499999999995</v>
+      </c>
+      <c r="D19" s="38">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="C20" s="36">
+        <v>0.70129870129870098</v>
+      </c>
+      <c r="D20" s="38">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="C21" s="31">
+        <v>0</v>
+      </c>
+      <c r="D21" s="38"/>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="28"/>
+      <c r="C28" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="37" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="C29" s="31">
+        <v>9.0909100000000007E-2</v>
+      </c>
+      <c r="D29" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" s="35" t="s">
+        <v>192</v>
+      </c>
+      <c r="C30" s="36">
+        <v>0.103896103896103</v>
+      </c>
+      <c r="D30" s="39">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="C31" s="36">
+        <v>5.1948099999999997E-2</v>
+      </c>
+      <c r="D31" s="38">
+        <v>2.6666666666666599E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="C32" s="36">
+        <v>5.1948051948051903E-2</v>
+      </c>
+      <c r="D32" s="38">
+        <v>4.6666699999999998E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="C33" s="33">
+        <v>0.42857143282890298</v>
+      </c>
+      <c r="D33" s="38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F946D1-EBA1-4976-A074-B5CA574C2B51}">
   <dimension ref="A2:A88"/>
   <sheetViews>
@@ -6022,206 +6257,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AF06F93-5909-4560-A480-0827EF86C188}">
-  <dimension ref="B4:D33"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="2:4">
-      <c r="B4" s="28"/>
-      <c r="C4" s="34" t="s">
-        <v>197</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4">
-      <c r="B5" s="28" t="s">
-        <v>191</v>
-      </c>
-      <c r="C5" s="32">
-        <v>0.62090000000000001</v>
-      </c>
-      <c r="D5" s="38"/>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="35" t="s">
-        <v>192</v>
-      </c>
-      <c r="C6" s="36">
-        <v>0.51948051948051899</v>
-      </c>
-      <c r="D6" s="39">
-        <v>0.793333333333333</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" s="35" t="s">
-        <v>193</v>
-      </c>
-      <c r="C7" s="36">
-        <v>0.57142899999999996</v>
-      </c>
-      <c r="D7" s="38">
-        <v>0.206666666666666</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" s="35" t="s">
-        <v>194</v>
-      </c>
-      <c r="C8" s="36">
-        <v>0.63636363636363602</v>
-      </c>
-      <c r="D8" s="38">
-        <v>0.793333333333333</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="B9" s="28" t="s">
-        <v>195</v>
-      </c>
-      <c r="C9" s="33">
-        <v>0.57142859697341897</v>
-      </c>
-      <c r="D9" s="38"/>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="B16" s="28"/>
-      <c r="C16" s="34" t="s">
-        <v>198</v>
-      </c>
-      <c r="D16" s="37" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="28" t="s">
-        <v>191</v>
-      </c>
-      <c r="C17" s="31">
-        <v>0.66990000000000005</v>
-      </c>
-      <c r="D17" s="38"/>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="35" t="s">
-        <v>192</v>
-      </c>
-      <c r="C18" s="36">
-        <v>0.70129870129870098</v>
-      </c>
-      <c r="D18" s="39">
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="35" t="s">
-        <v>193</v>
-      </c>
-      <c r="C19" s="36">
-        <v>0.67532499999999995</v>
-      </c>
-      <c r="D19" s="38">
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20" s="35" t="s">
-        <v>194</v>
-      </c>
-      <c r="C20" s="36">
-        <v>0.70129870129870098</v>
-      </c>
-      <c r="D20" s="38">
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="B21" s="28" t="s">
-        <v>195</v>
-      </c>
-      <c r="C21" s="31">
-        <v>0</v>
-      </c>
-      <c r="D21" s="38"/>
-    </row>
-    <row r="28" spans="2:4">
-      <c r="B28" s="28"/>
-      <c r="C28" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="D28" s="37" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4">
-      <c r="B29" s="28" t="s">
-        <v>191</v>
-      </c>
-      <c r="C29" s="31">
-        <v>7.5200000000000003E-2</v>
-      </c>
-      <c r="D29" s="38"/>
-    </row>
-    <row r="30" spans="2:4">
-      <c r="B30" s="35" t="s">
-        <v>192</v>
-      </c>
-      <c r="C30" s="36">
-        <v>0.103896103896103</v>
-      </c>
-      <c r="D30" s="39">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4">
-      <c r="B31" s="35" t="s">
-        <v>193</v>
-      </c>
-      <c r="C31" s="36">
-        <v>5.1948099999999997E-2</v>
-      </c>
-      <c r="D31" s="38">
-        <v>2.6666666666666599E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4">
-      <c r="B32" s="35" t="s">
-        <v>194</v>
-      </c>
-      <c r="C32" s="36">
-        <v>5.1948051948051903E-2</v>
-      </c>
-      <c r="D32" s="38">
-        <v>4.6666699999999998E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4">
-      <c r="B33" s="28" t="s">
-        <v>195</v>
-      </c>
-      <c r="C33" s="33">
-        <v>0.42857143282890298</v>
-      </c>
-      <c r="D33" s="38"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Retest Algorithm 5 with test data
</commit_message>
<xml_diff>
--- a/Table of article comparision.xlsx
+++ b/Table of article comparision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c49cb972183112a/Documents OneDrive/06 - CCT Masters in DA/Capstone - 2023/Capstone_Project_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="636" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{423AE944-4C86-480A-97AE-5B8FE3BF8CFD}"/>
+  <xr:revisionPtr revIDLastSave="640" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6579A2C9-D053-4F7E-A8A1-5368AD8129BA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
+    <workbookView xWindow="28965" yWindow="180" windowWidth="13395" windowHeight="13140" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison Chart" sheetId="1" r:id="rId1"/>
@@ -932,7 +932,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1017,6 +1017,12 @@
     <xf numFmtId="10" fontId="0" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1031,15 +1037,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4922,8 +4919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61403218-7A3E-4B26-8B7C-D3F4D407424F}">
   <dimension ref="A1:P82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20:M20"/>
+    <sheetView tabSelected="1" topLeftCell="J2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4937,7 +4934,7 @@
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" customWidth="1"/>
     <col min="10" max="10" width="40.85546875" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.85546875" customWidth="1"/>
     <col min="14" max="14" width="9.28515625" customWidth="1"/>
@@ -5112,16 +5109,16 @@
       <c r="C15">
         <v>0.57142857000000002</v>
       </c>
-      <c r="K15" s="41" t="s">
+      <c r="K15" s="43" t="s">
         <v>199</v>
       </c>
-      <c r="L15" s="42"/>
-      <c r="M15" s="43"/>
-      <c r="N15" s="44" t="s">
+      <c r="L15" s="44"/>
+      <c r="M15" s="45"/>
+      <c r="N15" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="O15" s="44"/>
-      <c r="P15" s="44"/>
+      <c r="O15" s="46"/>
+      <c r="P15" s="46"/>
     </row>
     <row r="16" spans="1:16">
       <c r="B16" s="8" t="s">
@@ -5181,7 +5178,7 @@
     </row>
     <row r="18" spans="1:16">
       <c r="B18" s="7"/>
-      <c r="J18" s="45" t="s">
+      <c r="J18" s="28" t="s">
         <v>192</v>
       </c>
       <c r="K18" s="33">
@@ -5213,7 +5210,7 @@
       <c r="C19" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="J19" s="45" t="s">
+      <c r="J19" s="28" t="s">
         <v>193</v>
       </c>
       <c r="K19" s="33">
@@ -5243,16 +5240,16 @@
         <v>60</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="J20" s="46" t="s">
+      <c r="J20" s="40" t="s">
         <v>194</v>
       </c>
-      <c r="K20" s="47">
+      <c r="K20" s="41">
         <v>0.63636363636363602</v>
       </c>
-      <c r="L20" s="47">
+      <c r="L20" s="41">
         <v>0.70129870129870098</v>
       </c>
-      <c r="M20" s="47">
+      <c r="M20" s="41">
         <v>5.1948051948051903E-2</v>
       </c>
       <c r="N20" s="38">
@@ -5281,9 +5278,15 @@
       <c r="M21" s="33">
         <v>0.42857143282890298</v>
       </c>
-      <c r="N21" s="38"/>
-      <c r="O21" s="38"/>
-      <c r="P21" s="38"/>
+      <c r="N21" s="38">
+        <v>0.79333335161209095</v>
+      </c>
+      <c r="O21" s="38">
+        <v>0</v>
+      </c>
+      <c r="P21" s="38">
+        <v>0.79333335161209095</v>
+      </c>
     </row>
     <row r="22" spans="1:16">
       <c r="B22" s="24" t="s">
@@ -5464,7 +5467,7 @@
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="40" t="s">
+      <c r="A45" s="42" t="s">
         <v>182</v>
       </c>
       <c r="B45" s="10" t="s">
@@ -5475,7 +5478,7 @@
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="40"/>
+      <c r="A46" s="42"/>
       <c r="B46" s="10" t="s">
         <v>90</v>
       </c>
@@ -5484,7 +5487,7 @@
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="40"/>
+      <c r="A47" s="42"/>
       <c r="B47" s="10" t="s">
         <v>91</v>
       </c>
@@ -5493,14 +5496,14 @@
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="40"/>
+      <c r="A48" s="42"/>
       <c r="B48" s="24" t="s">
         <v>77</v>
       </c>
       <c r="C48" s="11"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="40"/>
+      <c r="A49" s="42"/>
       <c r="B49" s="10" t="s">
         <v>91</v>
       </c>
@@ -5512,7 +5515,7 @@
       <c r="B50" s="10"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="40" t="s">
+      <c r="A51" s="42" t="s">
         <v>183</v>
       </c>
       <c r="B51" s="10" t="s">
@@ -5523,14 +5526,14 @@
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="40"/>
+      <c r="A52" s="42"/>
       <c r="B52" s="24" t="s">
         <v>77</v>
       </c>
       <c r="C52" s="11"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="40"/>
+      <c r="A53" s="42"/>
       <c r="B53" s="10" t="s">
         <v>91</v>
       </c>

</xml_diff>

<commit_message>
Completion of Chapt 6 & 7
</commit_message>
<xml_diff>
--- a/Table of article comparision.xlsx
+++ b/Table of article comparision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c49cb972183112a/Documents OneDrive/06 - CCT Masters in DA/Capstone - 2023/Capstone_Project_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="640" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6579A2C9-D053-4F7E-A8A1-5368AD8129BA}"/>
+  <xr:revisionPtr revIDLastSave="693" documentId="8_{810C794C-1EEA-42C5-8A1B-8BD049248668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97769090-7288-4E4F-9F5F-A345EA2C865D}"/>
   <bookViews>
-    <workbookView xWindow="28965" yWindow="180" windowWidth="13395" windowHeight="13140" activeTab="1" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
+    <workbookView xWindow="15150" yWindow="240" windowWidth="13395" windowHeight="15210" firstSheet="1" activeTab="2" xr2:uid="{CC8D71F3-3ABB-44FE-B655-1EBAB0F5AE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison Chart" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="210">
   <si>
     <t>Authors</t>
   </si>
@@ -688,12 +688,22 @@
   <si>
     <t>Algorithm 5 - Multi-Layer Perceptron (MLP)</t>
   </si>
+  <si>
+    <t>Loss</t>
+  </si>
+  <si>
+    <t>Initial Dataset</t>
+  </si>
+  <si>
+    <t>Test Dataset</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="10">
@@ -787,7 +797,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -927,12 +937,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1017,11 +1037,8 @@
     <xf numFmtId="10" fontId="0" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1038,8 +1055,18 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1278,6 +1305,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.793333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.79330000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1708,6 +1738,9 @@
                 <c:pt idx="3">
                   <c:v>0.92</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2001,7 +2034,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Graphing the Results '!$C$28</c:f>
+              <c:f>'Graphing the Results '!$C$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2022,7 +2055,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Graphing the Results '!$B$29:$B$33</c:f>
+              <c:f>'Graphing the Results '!$B$32:$B$36</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2045,7 +2078,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Graphing the Results '!$C$29:$C$33</c:f>
+              <c:f>'Graphing the Results '!$C$32:$C$36</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2078,7 +2111,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Graphing the Results '!$D$28</c:f>
+              <c:f>'Graphing the Results '!$D$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2099,7 +2132,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Graphing the Results '!$B$29:$B$33</c:f>
+              <c:f>'Graphing the Results '!$B$32:$B$36</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2122,7 +2155,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Graphing the Results '!$D$29:$D$33</c:f>
+              <c:f>'Graphing the Results '!$D$32:$D$36</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2137,6 +2170,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4.6666699999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.79330000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4205,7 +4241,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>348502</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>156882</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4235,13 +4271,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4919,8 +4955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61403218-7A3E-4B26-8B7C-D3F4D407424F}">
   <dimension ref="A1:P82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5109,16 +5145,16 @@
       <c r="C15">
         <v>0.57142857000000002</v>
       </c>
-      <c r="K15" s="43" t="s">
+      <c r="K15" s="42" t="s">
         <v>199</v>
       </c>
-      <c r="L15" s="44"/>
-      <c r="M15" s="45"/>
-      <c r="N15" s="46" t="s">
+      <c r="L15" s="43"/>
+      <c r="M15" s="44"/>
+      <c r="N15" s="45" t="s">
         <v>201</v>
       </c>
-      <c r="O15" s="46"/>
-      <c r="P15" s="46"/>
+      <c r="O15" s="45"/>
+      <c r="P15" s="45"/>
     </row>
     <row r="16" spans="1:16">
       <c r="B16" s="8" t="s">
@@ -5243,13 +5279,13 @@
       <c r="J20" s="40" t="s">
         <v>194</v>
       </c>
-      <c r="K20" s="41">
+      <c r="K20" s="33">
         <v>0.63636363636363602</v>
       </c>
-      <c r="L20" s="41">
+      <c r="L20" s="33">
         <v>0.70129870129870098</v>
       </c>
-      <c r="M20" s="41">
+      <c r="M20" s="33">
         <v>5.1948051948051903E-2</v>
       </c>
       <c r="N20" s="38">
@@ -5467,7 +5503,7 @@
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="42" t="s">
+      <c r="A45" s="41" t="s">
         <v>182</v>
       </c>
       <c r="B45" s="10" t="s">
@@ -5478,7 +5514,7 @@
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="42"/>
+      <c r="A46" s="41"/>
       <c r="B46" s="10" t="s">
         <v>90</v>
       </c>
@@ -5487,7 +5523,7 @@
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="42"/>
+      <c r="A47" s="41"/>
       <c r="B47" s="10" t="s">
         <v>91</v>
       </c>
@@ -5496,14 +5532,14 @@
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="42"/>
+      <c r="A48" s="41"/>
       <c r="B48" s="24" t="s">
         <v>77</v>
       </c>
       <c r="C48" s="11"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="42"/>
+      <c r="A49" s="41"/>
       <c r="B49" s="10" t="s">
         <v>91</v>
       </c>
@@ -5515,7 +5551,7 @@
       <c r="B50" s="10"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="42" t="s">
+      <c r="A51" s="41" t="s">
         <v>183</v>
       </c>
       <c r="B51" s="10" t="s">
@@ -5526,14 +5562,14 @@
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="42"/>
+      <c r="A52" s="41"/>
       <c r="B52" s="24" t="s">
         <v>77</v>
       </c>
       <c r="C52" s="11"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="42"/>
+      <c r="A53" s="41"/>
       <c r="B53" s="10" t="s">
         <v>91</v>
       </c>
@@ -5613,15 +5649,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AF06F93-5909-4560-A480-0827EF86C188}">
-  <dimension ref="B4:D33"/>
+  <dimension ref="B4:D36"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" customWidth="1"/>
@@ -5687,7 +5723,9 @@
       <c r="C9" s="33">
         <v>0.57142859697341897</v>
       </c>
-      <c r="D9" s="38"/>
+      <c r="D9" s="38">
+        <v>0.79330000000000001</v>
+      </c>
     </row>
     <row r="16" spans="2:4">
       <c r="B16" s="28"/>
@@ -5749,71 +5787,116 @@
       <c r="C21" s="31">
         <v>0</v>
       </c>
-      <c r="D21" s="38"/>
-    </row>
-    <row r="28" spans="2:4">
-      <c r="B28" s="28"/>
-      <c r="C28" s="34" t="s">
+      <c r="D21" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="48" t="s">
+        <v>195</v>
+      </c>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="28"/>
+      <c r="C24" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="D24" s="37" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="C25" s="47">
+        <v>-71067648</v>
+      </c>
+      <c r="D25" s="46">
+        <v>-4097.91162109375</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="31">
+        <v>0</v>
+      </c>
+      <c r="D26" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="28"/>
+      <c r="C31" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="D28" s="37" t="s">
+      <c r="D31" s="37" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="29" spans="2:4">
-      <c r="B29" s="28" t="s">
+    <row r="32" spans="2:4">
+      <c r="B32" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="C29" s="31">
+      <c r="C32" s="31">
         <v>9.0909100000000007E-2</v>
       </c>
-      <c r="D29" s="38">
+      <c r="D32" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:4">
-      <c r="B30" s="35" t="s">
+    <row r="33" spans="2:4">
+      <c r="B33" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="C30" s="36">
+      <c r="C33" s="36">
         <v>0.103896103896103</v>
       </c>
-      <c r="D30" s="39">
+      <c r="D33" s="39">
         <v>0.04</v>
       </c>
     </row>
-    <row r="31" spans="2:4">
-      <c r="B31" s="35" t="s">
+    <row r="34" spans="2:4">
+      <c r="B34" s="35" t="s">
         <v>193</v>
       </c>
-      <c r="C31" s="36">
+      <c r="C34" s="36">
         <v>5.1948099999999997E-2</v>
       </c>
-      <c r="D31" s="38">
+      <c r="D34" s="38">
         <v>2.6666666666666599E-2</v>
       </c>
     </row>
-    <row r="32" spans="2:4">
-      <c r="B32" s="35" t="s">
+    <row r="35" spans="2:4">
+      <c r="B35" s="35" t="s">
         <v>194</v>
       </c>
-      <c r="C32" s="36">
+      <c r="C35" s="36">
         <v>5.1948051948051903E-2</v>
       </c>
-      <c r="D32" s="38">
+      <c r="D35" s="38">
         <v>4.6666699999999998E-2</v>
       </c>
     </row>
-    <row r="33" spans="2:4">
-      <c r="B33" s="28" t="s">
+    <row r="36" spans="2:4">
+      <c r="B36" s="28" t="s">
         <v>206</v>
       </c>
-      <c r="C33" s="33">
+      <c r="C36" s="33">
         <v>0.42857143282890298</v>
       </c>
-      <c r="D33" s="38"/>
+      <c r="D36" s="38">
+        <v>0.79330000000000001</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B23:D23"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>